<commit_message>
List: pregnancies working. Children not there yet
</commit_message>
<xml_diff>
--- a/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
+++ b/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1590296F-57AB-4F5A-B63F-E5107D1FE4BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20E7AF3-1235-4843-93D7-D2B00E1AF702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="267">
   <si>
     <t>setting_name</t>
   </si>
@@ -257,9 +257,6 @@
     <t>required</t>
   </si>
   <si>
-    <t>Health centre area: {{data.HCNOME}}</t>
-  </si>
-  <si>
     <t>HCAREANOME</t>
   </si>
   <si>
@@ -272,24 +269,6 @@
     <t>REGNOME</t>
   </si>
   <si>
-    <t>Region: {{data.REGNOME}}</t>
-  </si>
-  <si>
-    <t>Subarea: {{data.SUBAREANOME}}</t>
-  </si>
-  <si>
-    <t>Village: {{data.TABNOME}}</t>
-  </si>
-  <si>
-    <t>Região: {{data.REGNOME}}</t>
-  </si>
-  <si>
-    <t>Área sanitárias: {{data.HCNOME}}</t>
-  </si>
-  <si>
-    <t>Tabanca: {{data.TABNOME}}</t>
-  </si>
-  <si>
     <t>NOMECRI</t>
   </si>
   <si>
@@ -524,18 +503,6 @@
     <t>Você está prestes a registrar uma nova criança em:</t>
   </si>
   <si>
-    <t>Household: {{data.MOR}}</t>
-  </si>
-  <si>
-    <t>Morança: {{data.MOR}}</t>
-  </si>
-  <si>
-    <t>Name of mother: {{data.NOME}}</t>
-  </si>
-  <si>
-    <t>Nome da mãe: {{data.NOME}}</t>
-  </si>
-  <si>
     <t>not(adate.hasUncertainty(data("DATASEG"))) &amp;&amp; data("DATASEG") != null &amp;&amp; adate.ageInYears(data("DATASEG")) != -9999 &amp;&amp; adate.ageInYears(data("DATASEG")) &lt; 2019</t>
   </si>
   <si>
@@ -813,6 +780,60 @@
   </si>
   <si>
     <t>Obrigado pelo seu tempo.</t>
+  </si>
+  <si>
+    <t>Region: &lt;b&gt;{{data.REGNOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Região: &lt;b&gt;{{data.REGNOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Health centre area: &lt;b&gt;{{data.HCAREANOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Área sanitárias: &lt;b&gt;{{data.HCAREANOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Subarea: &lt;b&gt;{{data.SUBAREANOME}}&lt;b&gt;</t>
+  </si>
+  <si>
+    <t>Subarea: &lt;b&gt;{{data.SUBAREANOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Village: &lt;b&gt;{{data.TABNOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Tabanca: &lt;b&gt;{{data.TABNOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Household: &lt;b&gt;{{data.MOR}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Morança: &lt;b&gt;{{data.MOR}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Name of mother: &lt;b&gt;{{data.NOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Nome da mãe: &lt;b&gt;{{data.NOME}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>GRAV</t>
+  </si>
+  <si>
+    <t>REGDIACRI</t>
+  </si>
+  <si>
+    <t>fu</t>
+  </si>
+  <si>
+    <t>POBCON</t>
+  </si>
+  <si>
+    <t>NUMESTCRI</t>
+  </si>
+  <si>
+    <t>instance_name</t>
   </si>
 </sst>
 </file>
@@ -884,12 +905,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -923,9 +950,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -944,6 +968,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1229,9 +1254,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,14 +1294,14 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>7122020</v>
       </c>
     </row>
@@ -1285,7 +1310,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1294,10 +1319,10 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1323,8 +1348,12 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B8" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G12:G24">
@@ -1339,9 +1368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:R111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G108" sqref="G108:H108"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,8 +1447,8 @@
       <c r="Q1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="9" t="s">
-        <v>160</v>
+      <c r="R1" s="8" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1432,10 +1461,10 @@
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H3" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1443,10 +1472,10 @@
         <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="H4" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1454,10 +1483,10 @@
         <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>249</v>
       </c>
       <c r="H5" t="s">
-        <v>82</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1465,21 +1494,21 @@
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>251</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="G7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" t="s">
-        <v>80</v>
+      <c r="G7" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1487,10 +1516,10 @@
         <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
+        <v>255</v>
       </c>
       <c r="H8" t="s">
-        <v>84</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1498,10 +1527,10 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>163</v>
+        <v>257</v>
       </c>
       <c r="H9" t="s">
-        <v>164</v>
+        <v>258</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -1512,10 +1541,10 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>165</v>
+        <v>259</v>
       </c>
       <c r="H10" t="s">
-        <v>166</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1533,10 +1562,10 @@
         <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H13" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1544,19 +1573,19 @@
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G14" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H14" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="P14" t="b">
         <v>0</v>
@@ -1577,10 +1606,10 @@
         <v>35</v>
       </c>
       <c r="G17" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H17" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -1588,10 +1617,10 @@
         <v>35</v>
       </c>
       <c r="G18" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="H18" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -1599,16 +1628,16 @@
         <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="F19" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="G19" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="H19" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="J19" t="b">
         <v>1</v>
@@ -1619,7 +1648,7 @@
         <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -1627,13 +1656,13 @@
         <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G21" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H21" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="J21" t="b">
         <v>1</v>
@@ -1656,10 +1685,10 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G25" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H25" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -1667,107 +1696,107 @@
         <v>35</v>
       </c>
       <c r="G26" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="H26" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="14" t="s">
+      <c r="C27" s="13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>214</v>
+      <c r="G28" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>203</v>
       </c>
       <c r="I28"/>
       <c r="J28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="14" t="s">
+    <row r="29" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
+    <row r="30" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="14" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="14" t="s">
+      <c r="C30" s="13" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G31" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>215</v>
+      <c r="G31" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>204</v>
       </c>
       <c r="I31"/>
       <c r="J31" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
+    <row r="32" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="13" t="s">
         <v>71</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
     </row>
-    <row r="33" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
+    <row r="33" spans="2:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="14" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D34" s="14" t="s">
+      <c r="C33" s="13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>216</v>
+      <c r="G34" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>205</v>
       </c>
       <c r="I34"/>
       <c r="J34" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
+    <row r="35" spans="2:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="13" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="14" t="s">
+    <row r="36" spans="2:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E36" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>205</v>
+      <c r="E36" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
@@ -1775,7 +1804,7 @@
         <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
@@ -1783,16 +1812,16 @@
         <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="F38" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G38" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H38" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="J38" t="b">
         <v>1</v>
@@ -1815,10 +1844,10 @@
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G42" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H42" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
@@ -1826,10 +1855,10 @@
         <v>35</v>
       </c>
       <c r="G43" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="H43" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
@@ -1837,16 +1866,16 @@
         <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="F44" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="G44" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="H44" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="J44" t="b">
         <v>1</v>
@@ -1857,7 +1886,7 @@
         <v>70</v>
       </c>
       <c r="C45" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
@@ -1865,19 +1894,19 @@
         <v>28</v>
       </c>
       <c r="F46" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="G46" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="H46" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="J46" t="b">
         <v>1</v>
       </c>
       <c r="K46" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="P46" t="b">
         <v>0</v>
@@ -1892,7 +1921,7 @@
       <c r="B48" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="12"/>
+      <c r="E48" s="11"/>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
@@ -1904,10 +1933,10 @@
         <v>35</v>
       </c>
       <c r="G50" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H50" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.25">
@@ -1918,13 +1947,13 @@
         <v>72</v>
       </c>
       <c r="F51" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G51" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H51" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="J51" t="b">
         <v>1</v>
@@ -1935,7 +1964,7 @@
         <v>70</v>
       </c>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
@@ -1943,16 +1972,16 @@
         <v>28</v>
       </c>
       <c r="F53" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G53" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="H53" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="K53" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="P53" t="b">
         <v>0</v>
@@ -1978,10 +2007,10 @@
         <v>35</v>
       </c>
       <c r="G57" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H57" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
@@ -1992,13 +2021,13 @@
         <v>56</v>
       </c>
       <c r="F58" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G58" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="H58" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="J58" t="b">
         <v>1</v>
@@ -2009,16 +2038,16 @@
         <v>53</v>
       </c>
       <c r="E59" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="F59" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G59" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H59" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="J59" t="b">
         <v>1</v>
@@ -2034,7 +2063,7 @@
         <v>70</v>
       </c>
       <c r="C61" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.25">
@@ -2047,10 +2076,10 @@
         <v>35</v>
       </c>
       <c r="G63" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H63" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.25">
@@ -2061,16 +2090,16 @@
         <v>55</v>
       </c>
       <c r="F64" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G64" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H64" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="K64" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="2:16" x14ac:dyDescent="0.25">
@@ -2078,7 +2107,7 @@
         <v>70</v>
       </c>
       <c r="C65" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="2:16" x14ac:dyDescent="0.25">
@@ -2086,16 +2115,16 @@
         <v>28</v>
       </c>
       <c r="F66" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G66" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="H66" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="K66" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="P66" t="b">
         <v>0</v>
@@ -2114,16 +2143,16 @@
         <v>55</v>
       </c>
       <c r="F68" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="G68" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H68" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="K68" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.25">
@@ -2131,7 +2160,7 @@
         <v>70</v>
       </c>
       <c r="C69" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="70" spans="2:16" x14ac:dyDescent="0.25">
@@ -2139,16 +2168,16 @@
         <v>28</v>
       </c>
       <c r="F70" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="G70" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="H70" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="K70" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="P70" t="b">
         <v>0</v>
@@ -2174,10 +2203,10 @@
         <v>35</v>
       </c>
       <c r="G74" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H74" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" spans="2:16" x14ac:dyDescent="0.25">
@@ -2188,16 +2217,16 @@
         <v>55</v>
       </c>
       <c r="F75" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="G75" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="H75" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="K75" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
     </row>
     <row r="76" spans="2:16" x14ac:dyDescent="0.25">
@@ -2210,7 +2239,7 @@
         <v>70</v>
       </c>
       <c r="C77" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
     </row>
     <row r="78" spans="2:16" x14ac:dyDescent="0.25">
@@ -2223,30 +2252,30 @@
         <v>35</v>
       </c>
       <c r="G79" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="H79" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="E80" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="F80" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="G80" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="H80" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="K80" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="81" spans="2:18" x14ac:dyDescent="0.25">
@@ -2254,16 +2283,16 @@
         <v>28</v>
       </c>
       <c r="F81" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="G81" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="H81" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="K81" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="2:18" x14ac:dyDescent="0.25">
@@ -2276,7 +2305,7 @@
         <v>70</v>
       </c>
       <c r="C83" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="84" spans="2:18" x14ac:dyDescent="0.25">
@@ -2289,36 +2318,36 @@
         <v>35</v>
       </c>
       <c r="G85" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H85" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="86" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D86" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="F86" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="G86" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="H86" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="K86" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="L86" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="M86" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="R86" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="2:18" x14ac:dyDescent="0.25">
@@ -2346,7 +2375,7 @@
         <v>70</v>
       </c>
       <c r="C91" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="92" spans="2:18" x14ac:dyDescent="0.25">
@@ -2359,10 +2388,10 @@
         <v>35</v>
       </c>
       <c r="G93" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H93" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="94" spans="2:18" x14ac:dyDescent="0.25">
@@ -2370,28 +2399,28 @@
         <v>49</v>
       </c>
       <c r="F94" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G94" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="H94" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="K94" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="L94" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="M94" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="N94" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="O94" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="2:18" x14ac:dyDescent="0.25">
@@ -2399,7 +2428,7 @@
         <v>70</v>
       </c>
       <c r="C95" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="2:18" x14ac:dyDescent="0.25">
@@ -2410,16 +2439,16 @@
         <v>55</v>
       </c>
       <c r="F96" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="G96" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="H96" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="K96" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="97" spans="2:16" x14ac:dyDescent="0.25">
@@ -2447,10 +2476,10 @@
         <v>35</v>
       </c>
       <c r="G101" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H101" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="102" spans="2:16" x14ac:dyDescent="0.25">
@@ -2461,13 +2490,13 @@
         <v>56</v>
       </c>
       <c r="F102" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G102" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="H102" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="J102" t="b">
         <v>1</v>
@@ -2478,7 +2507,7 @@
         <v>70</v>
       </c>
       <c r="C103" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="104" spans="2:16" x14ac:dyDescent="0.25">
@@ -2486,16 +2515,16 @@
         <v>28</v>
       </c>
       <c r="F104" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G104" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="H104" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="K104" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="P104" t="b">
         <v>0</v>
@@ -2521,10 +2550,10 @@
         <v>35</v>
       </c>
       <c r="G108" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="H108" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="109" spans="2:16" x14ac:dyDescent="0.25">
@@ -2532,10 +2561,10 @@
         <v>35</v>
       </c>
       <c r="G109" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="H109" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="110" spans="2:16" x14ac:dyDescent="0.25">
@@ -2543,10 +2572,10 @@
         <v>35</v>
       </c>
       <c r="G110" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="H110" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="111" spans="2:16" x14ac:dyDescent="0.25">
@@ -2591,1086 +2620,1086 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="B2" s="12" t="str">
+    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="11" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="B3" s="12" t="str">
+      <c r="C2" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="11" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="12" t="str">
+      <c r="C3" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+    </row>
+    <row r="5" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="11" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="C5" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="12" t="str">
+    </row>
+    <row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="11" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="12" t="str">
+      <c r="C6" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="11" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="12" t="str">
+    <row r="8" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+    </row>
+    <row r="9" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="11" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B10" s="12" t="str">
+      <c r="C9" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="11" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B11" s="12" t="str">
+      <c r="C10" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="11" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B12" s="12" t="str">
+      <c r="D11" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" s="11" t="str">
         <f>"33"</f>
         <v>33</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="14" t="str">
+      <c r="B14" s="13" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="14" t="str">
+      <c r="B15" s="13" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="14" t="str">
+      <c r="B16" s="13" t="str">
         <f>"5"</f>
         <v>5</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="14" t="str">
+      <c r="B17" s="13" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>131</v>
+      <c r="C17" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="14" t="str">
+      <c r="B18" s="13" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>132</v>
+      <c r="C18" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="14" t="str">
+      <c r="B20" s="13" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="14" t="str">
+      <c r="B21" s="13" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="14" t="str">
+      <c r="B23" s="13" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="14" t="str">
+      <c r="B24" s="13" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="13" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="14" t="str">
+      <c r="B25" s="13" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="13" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="14" t="str">
+      <c r="A27" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="13" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>122</v>
+      <c r="C27" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" s="14" t="str">
+      <c r="A28" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="13" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>123</v>
+      <c r="C28" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B29" s="14" t="str">
+      <c r="A29" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="13" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C29" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>124</v>
+      <c r="C29" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>222</v>
+      </c>
+      <c r="B31" t="s">
+        <v>231</v>
+      </c>
+      <c r="C31" t="s">
+        <v>232</v>
+      </c>
+      <c r="D31" t="s">
         <v>233</v>
       </c>
-      <c r="B31" t="s">
+    </row>
+    <row r="32" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" t="s">
+        <v>234</v>
+      </c>
+      <c r="C32" t="s">
+        <v>235</v>
+      </c>
+      <c r="D32" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>222</v>
+      </c>
+      <c r="B33" t="s">
+        <v>237</v>
+      </c>
+      <c r="C33" t="s">
+        <v>238</v>
+      </c>
+      <c r="D33" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>222</v>
+      </c>
+      <c r="B34" t="s">
+        <v>240</v>
+      </c>
+      <c r="C34" t="s">
+        <v>241</v>
+      </c>
+      <c r="D34" t="s">
         <v>242</v>
       </c>
-      <c r="C31" t="s">
+    </row>
+    <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>222</v>
+      </c>
+      <c r="B35" t="s">
         <v>243</v>
       </c>
-      <c r="D31" t="s">
+      <c r="C35" t="s">
+        <v>243</v>
+      </c>
+      <c r="D35" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>233</v>
-      </c>
-      <c r="B32" t="s">
-        <v>245</v>
-      </c>
-      <c r="C32" t="s">
-        <v>246</v>
-      </c>
-      <c r="D32" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>233</v>
-      </c>
-      <c r="B33" t="s">
-        <v>248</v>
-      </c>
-      <c r="C33" t="s">
-        <v>249</v>
-      </c>
-      <c r="D33" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>233</v>
-      </c>
-      <c r="B34" t="s">
-        <v>251</v>
-      </c>
-      <c r="C34" t="s">
-        <v>252</v>
-      </c>
-      <c r="D34" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>233</v>
-      </c>
-      <c r="B35" t="s">
-        <v>254</v>
-      </c>
-      <c r="C35" t="s">
-        <v>254</v>
-      </c>
-      <c r="D35" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-    </row>
-    <row r="38" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-    </row>
-    <row r="39" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-    </row>
-    <row r="40" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-    </row>
-    <row r="41" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
+    <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+    </row>
+    <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+    </row>
+    <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+    </row>
+    <row r="41" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="17"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="16"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="F43" s="14"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="F43" s="13"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
+      <c r="A48" s="13"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-    </row>
-    <row r="51" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-    </row>
-    <row r="52" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-    </row>
-    <row r="53" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-    </row>
-    <row r="54" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-    </row>
-    <row r="55" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+    </row>
+    <row r="51" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+    </row>
+    <row r="52" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+    </row>
+    <row r="53" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+    </row>
+    <row r="54" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+    </row>
+    <row r="55" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
+      <c r="A58" s="13"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="15"/>
+      <c r="A61" s="13"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
+      <c r="A62" s="13"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="15"/>
+      <c r="A63" s="13"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
+      <c r="A64" s="13"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
-      <c r="B65" s="18"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
+      <c r="A65" s="13"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
-      <c r="B66" s="18"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
+      <c r="A66" s="13"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="14"/>
-      <c r="B67" s="19"/>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20"/>
+      <c r="A67" s="13"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20"/>
+      <c r="A68" s="13"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
-      <c r="B69" s="19"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
+      <c r="A69" s="13"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
-      <c r="B70" s="19"/>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20"/>
+      <c r="A70" s="13"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
-      <c r="B71" s="19"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20"/>
+      <c r="A71" s="13"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
-      <c r="B72" s="19"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20"/>
+      <c r="A72" s="13"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
-      <c r="B73" s="19"/>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20"/>
+      <c r="A73" s="13"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
-      <c r="B74" s="19"/>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="19"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
-      <c r="B75" s="19"/>
-      <c r="C75" s="20"/>
-      <c r="D75" s="20"/>
+      <c r="A75" s="13"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
-      <c r="B76" s="19"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="20"/>
+      <c r="A76" s="13"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
-      <c r="B77" s="19"/>
-      <c r="C77" s="20"/>
-      <c r="D77" s="20"/>
+      <c r="A77" s="13"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="14"/>
-      <c r="B78" s="19"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="20"/>
+      <c r="A78" s="13"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="19"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
-      <c r="B79" s="19"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
+      <c r="A79" s="13"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
-      <c r="B80" s="19"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
+      <c r="A80" s="13"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
-      <c r="B81" s="19"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="20"/>
+      <c r="A81" s="13"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="19"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
-      <c r="B82" s="19"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20"/>
+      <c r="A82" s="13"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
-      <c r="B83" s="19"/>
-      <c r="C83" s="20"/>
-      <c r="D83" s="20"/>
+      <c r="A83" s="13"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
-      <c r="B84" s="19"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="20"/>
+      <c r="A84" s="13"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="19"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
-      <c r="B85" s="19"/>
-      <c r="C85" s="20"/>
-      <c r="D85" s="20"/>
+      <c r="A85" s="13"/>
+      <c r="B85" s="18"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
-      <c r="B86" s="19"/>
-      <c r="C86" s="20"/>
-      <c r="D86" s="20"/>
+      <c r="A86" s="13"/>
+      <c r="B86" s="18"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="19"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
-      <c r="B87" s="19"/>
-      <c r="C87" s="20"/>
-      <c r="D87" s="20"/>
+      <c r="A87" s="13"/>
+      <c r="B87" s="18"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="19"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="14"/>
-      <c r="B88" s="19"/>
-      <c r="C88" s="20"/>
-      <c r="D88" s="20"/>
+      <c r="A88" s="13"/>
+      <c r="B88" s="18"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
-      <c r="B89" s="18"/>
-      <c r="C89" s="15"/>
-      <c r="D89" s="15"/>
+      <c r="A89" s="13"/>
+      <c r="B89" s="17"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
-      <c r="B90" s="18"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="15"/>
+      <c r="A90" s="13"/>
+      <c r="B90" s="17"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
-      <c r="B91" s="18"/>
-      <c r="C91" s="20"/>
-      <c r="D91" s="20"/>
+      <c r="A91" s="13"/>
+      <c r="B91" s="17"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
-      <c r="B92" s="18"/>
-      <c r="C92" s="20"/>
-      <c r="D92" s="15"/>
+      <c r="A92" s="13"/>
+      <c r="B92" s="17"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="14"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="14"/>
-      <c r="B93" s="18"/>
-      <c r="C93" s="20"/>
-      <c r="D93" s="15"/>
+      <c r="A93" s="13"/>
+      <c r="B93" s="17"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="14"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="14"/>
-      <c r="B94" s="18"/>
-      <c r="C94" s="16"/>
-      <c r="D94" s="15"/>
+      <c r="A94" s="13"/>
+      <c r="B94" s="17"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="14"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
-      <c r="B95" s="18"/>
-      <c r="C95" s="16"/>
-      <c r="D95" s="15"/>
+      <c r="A95" s="13"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="14"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
-      <c r="B96" s="18"/>
-      <c r="C96" s="15"/>
-      <c r="D96" s="15"/>
+      <c r="A96" s="13"/>
+      <c r="B96" s="17"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="14"/>
-      <c r="B97" s="18"/>
-      <c r="C97" s="16"/>
-      <c r="D97" s="15"/>
+      <c r="A97" s="13"/>
+      <c r="B97" s="17"/>
+      <c r="C97" s="15"/>
+      <c r="D97" s="14"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
-      <c r="B98" s="18"/>
-      <c r="C98" s="16"/>
-      <c r="D98" s="15"/>
+      <c r="A98" s="13"/>
+      <c r="B98" s="17"/>
+      <c r="C98" s="15"/>
+      <c r="D98" s="14"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="14"/>
-      <c r="B99" s="18"/>
-      <c r="C99" s="16"/>
-      <c r="D99" s="15"/>
+      <c r="A99" s="13"/>
+      <c r="B99" s="17"/>
+      <c r="C99" s="15"/>
+      <c r="D99" s="14"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="14"/>
-      <c r="B100" s="18"/>
-      <c r="C100" s="16"/>
-      <c r="D100" s="15"/>
+      <c r="A100" s="13"/>
+      <c r="B100" s="17"/>
+      <c r="C100" s="15"/>
+      <c r="D100" s="14"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="14"/>
-      <c r="B101" s="18"/>
-      <c r="C101" s="16"/>
-      <c r="D101" s="15"/>
+      <c r="A101" s="13"/>
+      <c r="B101" s="17"/>
+      <c r="C101" s="15"/>
+      <c r="D101" s="14"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="14"/>
-      <c r="B102" s="18"/>
-      <c r="C102" s="16"/>
-      <c r="D102" s="15"/>
+      <c r="A102" s="13"/>
+      <c r="B102" s="17"/>
+      <c r="C102" s="15"/>
+      <c r="D102" s="14"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
-      <c r="B103" s="14"/>
-      <c r="C103" s="16"/>
-      <c r="D103" s="15"/>
+      <c r="A103" s="13"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="15"/>
+      <c r="D103" s="14"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
-      <c r="B104" s="14"/>
-      <c r="C104" s="16"/>
-      <c r="D104" s="15"/>
+      <c r="A104" s="13"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="15"/>
+      <c r="D104" s="14"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
-      <c r="B105" s="14"/>
-      <c r="C105" s="16"/>
-      <c r="D105" s="15"/>
+      <c r="A105" s="13"/>
+      <c r="B105" s="13"/>
+      <c r="C105" s="15"/>
+      <c r="D105" s="14"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
-      <c r="B106" s="14"/>
-      <c r="C106" s="16"/>
-      <c r="D106" s="15"/>
+      <c r="A106" s="13"/>
+      <c r="B106" s="13"/>
+      <c r="C106" s="15"/>
+      <c r="D106" s="14"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="14"/>
-      <c r="B107" s="18"/>
-      <c r="C107" s="16"/>
-      <c r="D107" s="15"/>
+      <c r="A107" s="13"/>
+      <c r="B107" s="17"/>
+      <c r="C107" s="15"/>
+      <c r="D107" s="14"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="14"/>
-      <c r="B108" s="18"/>
-      <c r="C108" s="16"/>
-      <c r="D108" s="15"/>
+      <c r="A108" s="13"/>
+      <c r="B108" s="17"/>
+      <c r="C108" s="15"/>
+      <c r="D108" s="14"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="14"/>
-      <c r="B109" s="14"/>
-      <c r="C109" s="16"/>
-      <c r="D109" s="15"/>
+      <c r="A109" s="13"/>
+      <c r="B109" s="13"/>
+      <c r="C109" s="15"/>
+      <c r="D109" s="14"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="14"/>
-      <c r="B110" s="14"/>
-      <c r="C110" s="16"/>
-      <c r="D110" s="15"/>
+      <c r="A110" s="13"/>
+      <c r="B110" s="13"/>
+      <c r="C110" s="15"/>
+      <c r="D110" s="14"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="14"/>
-      <c r="B111" s="18"/>
-      <c r="C111" s="16"/>
-      <c r="D111" s="15"/>
+      <c r="A111" s="13"/>
+      <c r="B111" s="17"/>
+      <c r="C111" s="15"/>
+      <c r="D111" s="14"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="14"/>
-      <c r="B112" s="14"/>
-      <c r="C112" s="16"/>
-      <c r="D112" s="15"/>
+      <c r="A112" s="13"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="15"/>
+      <c r="D112" s="14"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
-      <c r="B113" s="14"/>
-      <c r="C113" s="16"/>
-      <c r="D113" s="15"/>
+      <c r="A113" s="13"/>
+      <c r="B113" s="13"/>
+      <c r="C113" s="15"/>
+      <c r="D113" s="14"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="14"/>
-      <c r="B114" s="14"/>
-      <c r="C114" s="16"/>
-      <c r="D114" s="15"/>
+      <c r="A114" s="13"/>
+      <c r="B114" s="13"/>
+      <c r="C114" s="15"/>
+      <c r="D114" s="14"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
-      <c r="B115" s="18"/>
-      <c r="C115" s="16"/>
-      <c r="D115" s="15"/>
+      <c r="A115" s="13"/>
+      <c r="B115" s="17"/>
+      <c r="C115" s="15"/>
+      <c r="D115" s="14"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="14"/>
-      <c r="B116" s="14"/>
-      <c r="C116" s="16"/>
-      <c r="D116" s="15"/>
+      <c r="A116" s="13"/>
+      <c r="B116" s="13"/>
+      <c r="C116" s="15"/>
+      <c r="D116" s="14"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="14"/>
-      <c r="B117" s="14"/>
-      <c r="C117" s="16"/>
-      <c r="D117" s="15"/>
+      <c r="A117" s="13"/>
+      <c r="B117" s="13"/>
+      <c r="C117" s="15"/>
+      <c r="D117" s="14"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
-      <c r="B118" s="14"/>
-      <c r="C118" s="15"/>
-      <c r="D118" s="15"/>
+      <c r="A118" s="13"/>
+      <c r="B118" s="13"/>
+      <c r="C118" s="14"/>
+      <c r="D118" s="14"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
-      <c r="B119" s="18"/>
-      <c r="C119" s="16"/>
-      <c r="D119" s="15"/>
+      <c r="A119" s="13"/>
+      <c r="B119" s="17"/>
+      <c r="C119" s="15"/>
+      <c r="D119" s="14"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
-      <c r="B120" s="14"/>
-      <c r="C120" s="16"/>
-      <c r="D120" s="15"/>
+      <c r="A120" s="13"/>
+      <c r="B120" s="13"/>
+      <c r="C120" s="15"/>
+      <c r="D120" s="14"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
-      <c r="B121" s="14"/>
-      <c r="C121" s="16"/>
-      <c r="D121" s="15"/>
+      <c r="A121" s="13"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="15"/>
+      <c r="D121" s="14"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
-      <c r="B122" s="14"/>
-      <c r="C122" s="16"/>
-      <c r="D122" s="15"/>
+      <c r="A122" s="13"/>
+      <c r="B122" s="13"/>
+      <c r="C122" s="15"/>
+      <c r="D122" s="14"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="14"/>
-      <c r="B123" s="14"/>
-      <c r="C123" s="16"/>
-      <c r="D123" s="15"/>
+      <c r="A123" s="13"/>
+      <c r="B123" s="13"/>
+      <c r="C123" s="15"/>
+      <c r="D123" s="14"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
-      <c r="B124" s="18"/>
-      <c r="C124" s="16"/>
-      <c r="D124" s="15"/>
+      <c r="A124" s="13"/>
+      <c r="B124" s="17"/>
+      <c r="C124" s="15"/>
+      <c r="D124" s="14"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
-      <c r="B125" s="14"/>
-      <c r="C125" s="16"/>
-      <c r="D125" s="15"/>
+      <c r="A125" s="13"/>
+      <c r="B125" s="13"/>
+      <c r="C125" s="15"/>
+      <c r="D125" s="14"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="14"/>
-      <c r="B126" s="14"/>
-      <c r="C126" s="16"/>
-      <c r="D126" s="15"/>
+      <c r="A126" s="13"/>
+      <c r="B126" s="13"/>
+      <c r="C126" s="15"/>
+      <c r="D126" s="14"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
-      <c r="B127" s="14"/>
-      <c r="C127" s="15"/>
-      <c r="D127" s="15"/>
+      <c r="A127" s="13"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="14"/>
+      <c r="D127" s="14"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="14"/>
-      <c r="B128" s="14"/>
-      <c r="C128" s="15"/>
-      <c r="D128" s="15"/>
+      <c r="A128" s="13"/>
+      <c r="B128" s="13"/>
+      <c r="C128" s="14"/>
+      <c r="D128" s="14"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
-      <c r="B129" s="18"/>
-      <c r="C129" s="15"/>
-      <c r="D129" s="15"/>
+      <c r="A129" s="13"/>
+      <c r="B129" s="17"/>
+      <c r="C129" s="14"/>
+      <c r="D129" s="14"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="7"/>
+      <c r="B130" s="6"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B131" s="7"/>
+      <c r="B131" s="6"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B132" s="7"/>
+      <c r="B132" s="6"/>
       <c r="C132"/>
       <c r="D132"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B133" s="7"/>
+      <c r="B133" s="6"/>
       <c r="C133"/>
       <c r="D133"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="7"/>
+      <c r="B134" s="6"/>
       <c r="C134"/>
       <c r="D134"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B135" s="7"/>
+      <c r="B135" s="6"/>
       <c r="C135"/>
       <c r="D135"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B136" s="7"/>
+      <c r="B136" s="6"/>
       <c r="C136"/>
       <c r="D136"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" s="7"/>
+      <c r="B137" s="6"/>
       <c r="C137"/>
       <c r="D137"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="7"/>
+      <c r="B138" s="6"/>
       <c r="C138"/>
       <c r="D138"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B139" s="7"/>
+      <c r="B139" s="6"/>
       <c r="C139"/>
       <c r="D139"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="7"/>
+      <c r="B140" s="6"/>
       <c r="C140"/>
       <c r="D140"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B141" s="7"/>
+      <c r="B141" s="6"/>
       <c r="C141"/>
       <c r="D141"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B142" s="7"/>
+      <c r="B142" s="6"/>
       <c r="C142"/>
       <c r="D142"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B143" s="7"/>
+      <c r="B143" s="6"/>
       <c r="C143"/>
       <c r="D143"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B144" s="7"/>
+      <c r="B144" s="6"/>
       <c r="C144"/>
       <c r="D144"/>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B145" s="7"/>
+      <c r="B145" s="6"/>
       <c r="C145"/>
       <c r="D145"/>
     </row>
@@ -3697,19 +3726,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>220</v>
+      <c r="A2" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3736,16 +3765,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3771,11 +3800,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3813,7 +3842,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
@@ -3835,7 +3864,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
@@ -3857,7 +3886,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
         <v>63</v>
@@ -3879,7 +3908,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
         <v>63</v>
@@ -3901,7 +3930,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>261</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
@@ -3910,23 +3939,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" t="s">
         <v>63</v>
       </c>
-      <c r="C13" t="b">
+      <c r="C12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -3934,10 +3963,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -3945,10 +3974,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -3956,10 +3985,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>262</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -3967,10 +3996,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>265</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -3978,7 +4007,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
@@ -3987,23 +4016,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" t="b">
-        <v>0</v>
-      </c>
-    </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -4011,7 +4029,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>53</v>
@@ -4022,10 +4040,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -4033,7 +4051,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B25" t="s">
         <v>53</v>
@@ -4044,7 +4062,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
         <v>28</v>
@@ -4055,7 +4073,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>174</v>
+        <v>110</v>
       </c>
       <c r="B27" t="s">
         <v>53</v>
@@ -4066,10 +4084,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>179</v>
+        <v>85</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
+        <v>53</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -4077,7 +4095,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
@@ -4088,7 +4106,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
@@ -4099,10 +4117,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>163</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -4110,67 +4128,147 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>223</v>
       </c>
       <c r="B32" t="s">
+        <v>221</v>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>227</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>168</v>
+      </c>
+      <c r="B34" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" t="s">
         <v>53</v>
       </c>
-      <c r="C32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>97</v>
-      </c>
-      <c r="B33" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
         <v>28</v>
       </c>
-      <c r="C34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>202</v>
-      </c>
-      <c r="B36" t="s">
-        <v>53</v>
-      </c>
       <c r="C36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>205</v>
+        <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>206</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
         <v>53</v>
       </c>
       <c r="C38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>191</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>194</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>195</v>
+      </c>
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>264</v>
+      </c>
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to follow-up and variable names
</commit_message>
<xml_diff>
--- a/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
+++ b/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C17E3E-B453-48AD-86F3-2D50887B00FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A7956D-25DC-46E2-9D78-EDD7F0BE3BF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="272">
   <si>
     <t>setting_name</t>
   </si>
@@ -188,12 +188,6 @@
     <t>MOR</t>
   </si>
   <si>
-    <t>NOME</t>
-  </si>
-  <si>
-    <t>NUMEST</t>
-  </si>
-  <si>
     <t>select_one</t>
   </si>
   <si>
@@ -284,21 +278,12 @@
     <t>BCGDATA</t>
   </si>
   <si>
-    <t>POLIO0</t>
-  </si>
-  <si>
-    <t>POLIO0DATA</t>
-  </si>
-  <si>
     <t>VACINFO</t>
   </si>
   <si>
     <t>ESTADOCRI</t>
   </si>
   <si>
-    <t>DATASAI</t>
-  </si>
-  <si>
     <t>MUAC</t>
   </si>
   <si>
@@ -515,9 +500,6 @@
     <t>Data de mudança / morte</t>
   </si>
   <si>
-    <t>(data("ESTADOCRI") != 2 &amp;&amp; data("ESTADOCRI") != 3) || ((data("ESTADOCRI") == 2 || data("ESTADOCRI") == 3) &amp;&amp; data("DATASAI") != null &amp;&amp; adate.ageInYears(data("DATASAI")) != -9999 &amp;&amp; adate.ageInYears(data("DATASAI")) &lt; 2019)</t>
-  </si>
-  <si>
     <t>data("BCG") != null || data("VACINAS") !=1</t>
   </si>
   <si>
@@ -578,9 +560,6 @@
     <t>(data("HOSPDATA") != null &amp;&amp; adate.ageInYears(data("HOSPDATA")) != -9999 &amp;&amp; adate.ageInYears(data("HOSPDATA")) &lt; 2019) || data("HOSP") != 1</t>
   </si>
   <si>
-    <t>VISNO</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Follow-up on child {{data.NOMECRI}}&lt;/b&gt;</t>
   </si>
   <si>
@@ -809,31 +788,67 @@
     <t>Morança: &lt;b&gt;{{data.MOR}}&lt;/b&gt;</t>
   </si>
   <si>
-    <t>Name of mother: &lt;b&gt;{{data.NOME}}&lt;/b&gt;</t>
-  </si>
-  <si>
-    <t>Nome da mãe: &lt;b&gt;{{data.NOME}}&lt;/b&gt;</t>
-  </si>
-  <si>
     <t>GRAV</t>
   </si>
   <si>
-    <t>REGDIACRI</t>
-  </si>
-  <si>
-    <t>fu</t>
-  </si>
-  <si>
     <t>POBCON</t>
   </si>
   <si>
-    <t>NUMESTCRI</t>
-  </si>
-  <si>
     <t>instance_name</t>
   </si>
   <si>
     <t>data("BCGREACT") != null || data("BCG") != 1 || data('ESTADOCRI') != 1</t>
+  </si>
+  <si>
+    <t>DATASAICRI</t>
+  </si>
+  <si>
+    <t>Name of mother: &lt;b&gt;{{data.NOMEMUL}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>Nome da mãe: &lt;b&gt;{{data.NOMEMUL}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>(data("ESTADOCRI") != 2 &amp;&amp; data("ESTADOCRI") != 3) || ((data("ESTADOCRI") == 2 || data("ESTADOCRI") == 3) &amp;&amp; data("DATASAICRI") != null &amp;&amp; adate.ageInYears(data("DATASAICRI")) != -9999 &amp;&amp; adate.ageInYears(data("DATASAICRI")) &lt; 2019)</t>
+  </si>
+  <si>
+    <t>ESTADOMUL</t>
+  </si>
+  <si>
+    <t>Status of woman</t>
+  </si>
+  <si>
+    <t>Estado de mulher</t>
+  </si>
+  <si>
+    <t>data("ESTADOMUL") == "2" || data("ESTADOMUL") == "3"</t>
+  </si>
+  <si>
+    <t>DATASAIMUL</t>
+  </si>
+  <si>
+    <t>(data("ESTADOMUL") != 2 &amp;&amp; data("ESTADOMUL") != 3) || ((data("ESTADOMUL") == 2 || data("ESTADOMUL") == 3) &amp;&amp; data("DATASAIMUL") != null &amp;&amp; adate.ageInYears(data("DATASAIMUL")) != -9999 &amp;&amp; adate.ageInYears(data("DATASAIMUL")) &lt; 2019)</t>
+  </si>
+  <si>
+    <t>From MUL</t>
+  </si>
+  <si>
+    <t>VISNOCRI</t>
+  </si>
+  <si>
+    <t>IDMUL</t>
+  </si>
+  <si>
+    <t>NOMEMUL</t>
+  </si>
+  <si>
+    <t>IDCRI</t>
+  </si>
+  <si>
+    <t>First visit</t>
+  </si>
+  <si>
+    <t>FU</t>
   </si>
 </sst>
 </file>
@@ -1294,7 +1309,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1310,7 +1325,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1319,10 +1334,10 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1349,10 +1364,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1366,11 +1381,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:R111"/>
+  <dimension ref="A1:R118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K96" sqref="K96"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,7 +1439,7 @@
         <v>22</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>39</v>
@@ -1448,7 +1463,7 @@
         <v>44</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1461,10 +1476,10 @@
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H3" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1472,10 +1487,10 @@
         <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="H4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1483,10 +1498,10 @@
         <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="H5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1494,10 +1509,10 @@
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="H6" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1505,10 +1520,10 @@
         <v>35</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1516,10 +1531,10 @@
         <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="H8" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1527,10 +1542,10 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="H9" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -1541,10 +1556,10 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1562,10 +1577,10 @@
         <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H13" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1573,19 +1588,19 @@
         <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G14" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H14" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="P14" t="b">
         <v>0</v>
@@ -1601,102 +1616,111 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>35</v>
       </c>
       <c r="G17" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H17" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" t="s">
+        <v>259</v>
+      </c>
+      <c r="G18" t="s">
+        <v>260</v>
+      </c>
+      <c r="H18" t="s">
+        <v>261</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
+        <v>263</v>
+      </c>
+      <c r="G20" t="s">
+        <v>153</v>
+      </c>
+      <c r="H20" t="s">
+        <v>154</v>
+      </c>
+      <c r="K20" t="s">
+        <v>264</v>
+      </c>
+      <c r="P20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
         <v>35</v>
       </c>
-      <c r="G18" t="s">
-        <v>184</v>
-      </c>
-      <c r="H18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" t="s">
-        <v>186</v>
-      </c>
-      <c r="F19" t="s">
-        <v>190</v>
-      </c>
-      <c r="G19" t="s">
-        <v>191</v>
-      </c>
-      <c r="H19" t="s">
-        <v>192</v>
-      </c>
-      <c r="J19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C20" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F21" t="s">
-        <v>78</v>
-      </c>
-      <c r="G21" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" t="s">
-        <v>94</v>
-      </c>
-      <c r="J21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>175</v>
+      </c>
+      <c r="H24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>35</v>
       </c>
       <c r="G25" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="H25" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" t="s">
+        <v>179</v>
+      </c>
+      <c r="F26" t="s">
         <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
-        <v>35</v>
       </c>
       <c r="G26" t="s">
         <v>184</v>
@@ -1704,234 +1728,221 @@
       <c r="H26" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="27" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="H28" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="I28"/>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" t="s">
+        <v>88</v>
+      </c>
+      <c r="H28" t="s">
+        <v>89</v>
+      </c>
       <c r="J28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D31" s="13" t="s">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
         <v>35</v>
       </c>
-      <c r="G31" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="I31"/>
-      <c r="J31" t="b">
+      <c r="G32" t="s">
+        <v>175</v>
+      </c>
+      <c r="H32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" t="s">
+        <v>177</v>
+      </c>
+      <c r="H33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="I35"/>
+      <c r="J35" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="I32"/>
-      <c r="J32"/>
-    </row>
-    <row r="33" spans="2:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D34" s="13" t="s">
+    <row r="36" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="H34" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="I34"/>
-      <c r="J34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="2:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="F36" s="13" t="s">
+      <c r="G38" s="13" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>53</v>
-      </c>
-      <c r="E38" t="s">
-        <v>96</v>
-      </c>
-      <c r="F38" t="s">
-        <v>79</v>
-      </c>
-      <c r="G38" t="s">
-        <v>96</v>
-      </c>
-      <c r="H38" t="s">
-        <v>97</v>
-      </c>
+      <c r="H38" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="I38"/>
       <c r="J38" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="39" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I39"/>
+      <c r="J39"/>
+    </row>
+    <row r="40" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="I41"/>
+      <c r="J41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" t="s">
+        <v>77</v>
+      </c>
+      <c r="G45" t="s">
+        <v>91</v>
+      </c>
+      <c r="H45" t="s">
+        <v>92</v>
+      </c>
+      <c r="J45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
         <v>35</v>
       </c>
-      <c r="G42" t="s">
-        <v>182</v>
-      </c>
-      <c r="H42" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
-        <v>35</v>
-      </c>
-      <c r="G43" t="s">
-        <v>184</v>
-      </c>
-      <c r="H43" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E44" t="s">
-        <v>186</v>
-      </c>
-      <c r="F44" t="s">
-        <v>194</v>
-      </c>
-      <c r="G44" t="s">
-        <v>195</v>
-      </c>
-      <c r="H44" t="s">
-        <v>196</v>
-      </c>
-      <c r="J44" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
-        <v>28</v>
-      </c>
-      <c r="F46" t="s">
-        <v>80</v>
-      </c>
-      <c r="G46" t="s">
-        <v>98</v>
-      </c>
-      <c r="H46" t="s">
-        <v>99</v>
-      </c>
-      <c r="J46" t="b">
-        <v>1</v>
-      </c>
-      <c r="K46" t="s">
-        <v>157</v>
-      </c>
-      <c r="P46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>38</v>
-      </c>
-      <c r="E48" s="11"/>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>37</v>
+      <c r="G49" t="s">
+        <v>175</v>
+      </c>
+      <c r="H49" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.25">
@@ -1939,27 +1950,27 @@
         <v>35</v>
       </c>
       <c r="G50" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="H50" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E51" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="F51" t="s">
-        <v>86</v>
+        <v>187</v>
       </c>
       <c r="G51" t="s">
-        <v>95</v>
+        <v>188</v>
       </c>
       <c r="H51" t="s">
-        <v>127</v>
+        <v>189</v>
       </c>
       <c r="J51" t="b">
         <v>1</v>
@@ -1967,10 +1978,10 @@
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C52" t="s">
-        <v>128</v>
+        <v>198</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
@@ -1978,16 +1989,19 @@
         <v>28</v>
       </c>
       <c r="F53" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="G53" t="s">
-        <v>158</v>
+        <v>93</v>
       </c>
       <c r="H53" t="s">
-        <v>159</v>
+        <v>94</v>
+      </c>
+      <c r="J53" t="b">
+        <v>1</v>
       </c>
       <c r="K53" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="P53" t="b">
         <v>0</v>
@@ -1995,13 +2009,14 @@
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>38</v>
       </c>
+      <c r="E55" s="11"/>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
@@ -2013,537 +2028,537 @@
         <v>35</v>
       </c>
       <c r="G57" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H57" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E58" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="F58" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="G58" t="s">
-        <v>118</v>
+        <v>90</v>
       </c>
       <c r="H58" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="J58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
-        <v>53</v>
-      </c>
-      <c r="E59" t="s">
-        <v>111</v>
-      </c>
-      <c r="F59" t="s">
-        <v>85</v>
-      </c>
-      <c r="G59" t="s">
-        <v>120</v>
-      </c>
-      <c r="H59" t="s">
-        <v>121</v>
-      </c>
-      <c r="J59" t="b">
-        <v>1</v>
+      <c r="B59" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>38</v>
+      <c r="D60" t="s">
+        <v>28</v>
+      </c>
+      <c r="F60" t="s">
+        <v>255</v>
+      </c>
+      <c r="G60" t="s">
+        <v>153</v>
+      </c>
+      <c r="H60" t="s">
+        <v>154</v>
+      </c>
+      <c r="K60" t="s">
+        <v>258</v>
+      </c>
+      <c r="P60" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>70</v>
-      </c>
-      <c r="C61" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
-        <v>35</v>
-      </c>
-      <c r="G63" t="s">
-        <v>182</v>
-      </c>
-      <c r="H63" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>53</v>
-      </c>
-      <c r="E64" t="s">
-        <v>55</v>
-      </c>
-      <c r="F64" t="s">
-        <v>81</v>
+        <v>35</v>
       </c>
       <c r="G64" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="H64" t="s">
-        <v>135</v>
-      </c>
-      <c r="K64" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>70</v>
-      </c>
-      <c r="C65" t="s">
-        <v>137</v>
+      <c r="D65" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65" t="s">
+        <v>54</v>
+      </c>
+      <c r="F65" t="s">
+        <v>105</v>
+      </c>
+      <c r="G65" t="s">
+        <v>113</v>
+      </c>
+      <c r="H65" t="s">
+        <v>114</v>
+      </c>
+      <c r="J65" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="E66" t="s">
+        <v>106</v>
       </c>
       <c r="F66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G66" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="H66" t="s">
-        <v>139</v>
-      </c>
-      <c r="K66" t="s">
-        <v>162</v>
-      </c>
-      <c r="P66" t="b">
-        <v>0</v>
+        <v>116</v>
+      </c>
+      <c r="J66" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
-        <v>53</v>
-      </c>
-      <c r="E68" t="s">
-        <v>55</v>
-      </c>
-      <c r="F68" t="s">
-        <v>212</v>
-      </c>
-      <c r="G68" t="s">
-        <v>140</v>
-      </c>
-      <c r="H68" t="s">
-        <v>141</v>
-      </c>
-      <c r="K68" t="s">
-        <v>214</v>
+      <c r="B68" t="s">
+        <v>68</v>
+      </c>
+      <c r="C68" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>70</v>
-      </c>
-      <c r="C69" t="s">
-        <v>211</v>
+        <v>37</v>
       </c>
     </row>
     <row r="70" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
-        <v>28</v>
-      </c>
-      <c r="F70" t="s">
-        <v>213</v>
+        <v>35</v>
       </c>
       <c r="G70" t="s">
-        <v>138</v>
+        <v>175</v>
       </c>
       <c r="H70" t="s">
-        <v>139</v>
-      </c>
-      <c r="K70" t="s">
-        <v>215</v>
-      </c>
-      <c r="P70" t="b">
-        <v>0</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>71</v>
+      <c r="D71" t="s">
+        <v>51</v>
+      </c>
+      <c r="E71" t="s">
+        <v>53</v>
+      </c>
+      <c r="F71" t="s">
+        <v>79</v>
+      </c>
+      <c r="G71" t="s">
+        <v>131</v>
+      </c>
+      <c r="H71" t="s">
+        <v>130</v>
+      </c>
+      <c r="K71" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>38</v>
+        <v>68</v>
+      </c>
+      <c r="C72" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="73" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>37</v>
+      <c r="D73" t="s">
+        <v>28</v>
+      </c>
+      <c r="F73" t="s">
+        <v>80</v>
+      </c>
+      <c r="G73" t="s">
+        <v>133</v>
+      </c>
+      <c r="H73" t="s">
+        <v>134</v>
+      </c>
+      <c r="K73" t="s">
+        <v>156</v>
+      </c>
+      <c r="P73" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>35</v>
-      </c>
-      <c r="G74" t="s">
-        <v>182</v>
-      </c>
-      <c r="H74" t="s">
-        <v>183</v>
+      <c r="B74" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
+        <v>51</v>
+      </c>
+      <c r="E75" t="s">
         <v>53</v>
       </c>
-      <c r="E75" t="s">
-        <v>55</v>
-      </c>
       <c r="F75" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="G75" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="H75" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="K75" t="s">
-        <v>166</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>38</v>
+        <v>68</v>
+      </c>
+      <c r="C76" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>70</v>
-      </c>
-      <c r="C77" t="s">
-        <v>217</v>
+      <c r="D77" t="s">
+        <v>28</v>
+      </c>
+      <c r="F77" t="s">
+        <v>206</v>
+      </c>
+      <c r="G77" t="s">
+        <v>133</v>
+      </c>
+      <c r="H77" t="s">
+        <v>134</v>
+      </c>
+      <c r="K77" t="s">
+        <v>208</v>
+      </c>
+      <c r="P77" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D79" t="s">
-        <v>35</v>
-      </c>
-      <c r="G79" t="s">
-        <v>218</v>
-      </c>
-      <c r="H79" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D80" t="s">
-        <v>220</v>
-      </c>
-      <c r="E80" t="s">
-        <v>221</v>
-      </c>
-      <c r="F80" t="s">
-        <v>222</v>
-      </c>
-      <c r="G80" t="s">
-        <v>223</v>
-      </c>
-      <c r="H80" t="s">
-        <v>224</v>
-      </c>
-      <c r="K80" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="81" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
-        <v>28</v>
-      </c>
-      <c r="F81" t="s">
-        <v>226</v>
+        <v>35</v>
       </c>
       <c r="G81" t="s">
-        <v>227</v>
+        <v>175</v>
       </c>
       <c r="H81" t="s">
-        <v>228</v>
-      </c>
-      <c r="K81" t="s">
-        <v>229</v>
+        <v>176</v>
       </c>
     </row>
     <row r="82" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>38</v>
+      <c r="D82" t="s">
+        <v>51</v>
+      </c>
+      <c r="E82" t="s">
+        <v>53</v>
+      </c>
+      <c r="F82" t="s">
+        <v>157</v>
+      </c>
+      <c r="G82" t="s">
+        <v>158</v>
+      </c>
+      <c r="H82" t="s">
+        <v>159</v>
+      </c>
+      <c r="K82" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="83" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>70</v>
-      </c>
-      <c r="C83" t="s">
-        <v>216</v>
+        <v>38</v>
       </c>
     </row>
     <row r="84" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
+        <v>68</v>
+      </c>
+      <c r="C84" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D85" t="s">
-        <v>35</v>
-      </c>
-      <c r="G85" t="s">
-        <v>182</v>
-      </c>
-      <c r="H85" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="86" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D86" t="s">
-        <v>167</v>
-      </c>
-      <c r="F86" t="s">
-        <v>168</v>
+        <v>35</v>
       </c>
       <c r="G86" t="s">
-        <v>169</v>
+        <v>211</v>
       </c>
       <c r="H86" t="s">
-        <v>170</v>
-      </c>
-      <c r="K86" t="s">
-        <v>171</v>
-      </c>
-      <c r="L86" t="s">
-        <v>172</v>
-      </c>
-      <c r="M86" t="s">
-        <v>173</v>
-      </c>
-      <c r="R86" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
     </row>
     <row r="87" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>38</v>
+      <c r="D87" t="s">
+        <v>213</v>
+      </c>
+      <c r="E87" t="s">
+        <v>214</v>
+      </c>
+      <c r="F87" t="s">
+        <v>215</v>
+      </c>
+      <c r="G87" t="s">
+        <v>216</v>
+      </c>
+      <c r="H87" t="s">
+        <v>217</v>
+      </c>
+      <c r="K87" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="88" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>71</v>
+      <c r="D88" t="s">
+        <v>28</v>
+      </c>
+      <c r="F88" t="s">
+        <v>219</v>
+      </c>
+      <c r="G88" t="s">
+        <v>220</v>
+      </c>
+      <c r="H88" t="s">
+        <v>221</v>
+      </c>
+      <c r="K88" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="89" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="90" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="C90" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="91" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>70</v>
-      </c>
-      <c r="C91" t="s">
-        <v>129</v>
+        <v>37</v>
       </c>
     </row>
     <row r="92" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>37</v>
+      <c r="D92" t="s">
+        <v>35</v>
+      </c>
+      <c r="G92" t="s">
+        <v>175</v>
+      </c>
+      <c r="H92" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="93" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D93" t="s">
-        <v>35</v>
+        <v>161</v>
+      </c>
+      <c r="F93" t="s">
+        <v>162</v>
       </c>
       <c r="G93" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="H93" t="s">
-        <v>183</v>
+        <v>164</v>
+      </c>
+      <c r="K93" t="s">
+        <v>165</v>
+      </c>
+      <c r="L93" t="s">
+        <v>166</v>
+      </c>
+      <c r="M93" t="s">
+        <v>167</v>
+      </c>
+      <c r="R93" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="94" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D94" t="s">
-        <v>49</v>
-      </c>
-      <c r="F94" t="s">
-        <v>88</v>
-      </c>
-      <c r="G94" t="s">
-        <v>133</v>
-      </c>
-      <c r="H94" t="s">
-        <v>134</v>
-      </c>
-      <c r="K94" t="s">
-        <v>175</v>
-      </c>
-      <c r="L94" t="s">
-        <v>176</v>
-      </c>
-      <c r="M94" t="s">
-        <v>177</v>
-      </c>
-      <c r="N94" t="s">
-        <v>178</v>
-      </c>
-      <c r="O94" t="s">
-        <v>179</v>
+      <c r="B94" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="95" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>70</v>
-      </c>
-      <c r="C95" t="s">
-        <v>130</v>
+        <v>69</v>
       </c>
     </row>
     <row r="96" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D96" t="s">
-        <v>53</v>
-      </c>
-      <c r="E96" t="s">
-        <v>55</v>
-      </c>
-      <c r="F96" t="s">
-        <v>89</v>
-      </c>
-      <c r="G96" t="s">
-        <v>131</v>
-      </c>
-      <c r="H96" t="s">
-        <v>132</v>
-      </c>
-      <c r="K96" t="s">
-        <v>266</v>
+      <c r="B96" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="97" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="98" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>38</v>
+        <v>68</v>
+      </c>
+      <c r="C98" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="99" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>37</v>
+      <c r="D100" t="s">
+        <v>35</v>
+      </c>
+      <c r="G100" t="s">
+        <v>175</v>
+      </c>
+      <c r="H100" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="101" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D101" t="s">
-        <v>35</v>
+        <v>49</v>
+      </c>
+      <c r="F101" t="s">
+        <v>83</v>
       </c>
       <c r="G101" t="s">
-        <v>182</v>
+        <v>128</v>
       </c>
       <c r="H101" t="s">
-        <v>183</v>
+        <v>129</v>
+      </c>
+      <c r="K101" t="s">
+        <v>169</v>
+      </c>
+      <c r="L101" t="s">
+        <v>170</v>
+      </c>
+      <c r="M101" t="s">
+        <v>171</v>
+      </c>
+      <c r="N101" t="s">
+        <v>172</v>
+      </c>
+      <c r="O101" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="102" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D102" t="s">
+      <c r="B102" t="s">
+        <v>68</v>
+      </c>
+      <c r="C102" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>51</v>
+      </c>
+      <c r="E103" t="s">
         <v>53</v>
       </c>
-      <c r="E102" t="s">
-        <v>56</v>
-      </c>
-      <c r="F102" t="s">
-        <v>90</v>
-      </c>
-      <c r="G102" t="s">
-        <v>142</v>
-      </c>
-      <c r="H102" t="s">
-        <v>146</v>
-      </c>
-      <c r="J102" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B103" t="s">
-        <v>70</v>
-      </c>
-      <c r="C103" t="s">
-        <v>143</v>
+      <c r="F103" t="s">
+        <v>84</v>
+      </c>
+      <c r="G103" t="s">
+        <v>126</v>
+      </c>
+      <c r="H103" t="s">
+        <v>127</v>
+      </c>
+      <c r="K103" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="104" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D104" t="s">
-        <v>28</v>
-      </c>
-      <c r="F104" t="s">
-        <v>91</v>
-      </c>
-      <c r="G104" t="s">
-        <v>144</v>
-      </c>
-      <c r="H104" t="s">
-        <v>145</v>
-      </c>
-      <c r="K104" t="s">
-        <v>180</v>
-      </c>
-      <c r="P104" t="b">
-        <v>0</v>
+      <c r="B104" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="105" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
     </row>
     <row r="107" spans="2:16" x14ac:dyDescent="0.25">
@@ -2556,36 +2571,110 @@
         <v>35</v>
       </c>
       <c r="G108" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H108" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="109" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
+        <v>51</v>
+      </c>
+      <c r="E109" t="s">
+        <v>54</v>
+      </c>
+      <c r="F109" t="s">
+        <v>85</v>
+      </c>
+      <c r="G109" t="s">
+        <v>137</v>
+      </c>
+      <c r="H109" t="s">
+        <v>141</v>
+      </c>
+      <c r="J109" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>68</v>
+      </c>
+      <c r="C110" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>28</v>
+      </c>
+      <c r="F111" t="s">
+        <v>86</v>
+      </c>
+      <c r="G111" t="s">
+        <v>139</v>
+      </c>
+      <c r="H111" t="s">
+        <v>140</v>
+      </c>
+      <c r="K111" t="s">
+        <v>174</v>
+      </c>
+      <c r="P111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
         <v>35</v>
       </c>
-      <c r="G109" t="s">
-        <v>244</v>
-      </c>
-      <c r="H109" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="110" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D110" t="s">
+      <c r="G115" t="s">
+        <v>175</v>
+      </c>
+      <c r="H115" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
         <v>35</v>
       </c>
-      <c r="G110" t="s">
-        <v>246</v>
-      </c>
-      <c r="H110" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="111" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
+      <c r="G116" t="s">
+        <v>237</v>
+      </c>
+      <c r="H116" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>35</v>
+      </c>
+      <c r="G117" t="s">
+        <v>239</v>
+      </c>
+      <c r="H117" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2600,7 +2689,7 @@
   <dimension ref="A1:F145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
@@ -2628,32 +2717,32 @@
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B2" s="11" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B3" s="11" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2664,47 +2753,47 @@
     </row>
     <row r="5" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B5" s="11" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B6" s="11" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B7" s="11" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2715,62 +2804,62 @@
     </row>
     <row r="9" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B9" s="11" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B10" s="11" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B11" s="11" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B12" s="11" t="str">
         <f>"33"</f>
         <v>33</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2781,77 +2870,77 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B14" s="13" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B15" s="13" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B16" s="13" t="str">
         <f>"5"</f>
         <v>5</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B17" s="13" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B18" s="13" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2862,32 +2951,32 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20" s="13" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" s="13" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2898,47 +2987,47 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="13" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="13" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" s="13" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2949,47 +3038,47 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B27" s="13" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B28" s="13" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B29" s="13" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3000,72 +3089,72 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B31" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C31" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D31" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B32" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="C32" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D32" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B33" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C33" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D33" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B34" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="C34" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D34" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B35" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C35" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D35" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3741,10 +3830,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3806,11 +3895,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3845,13 +3934,16 @@
       <c r="C2" t="b">
         <v>0</v>
       </c>
+      <c r="D2" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -3870,10 +3962,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -3892,10 +3984,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -3914,10 +4006,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -3928,7 +4020,7 @@
         <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -3936,7 +4028,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
@@ -3947,10 +4039,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>266</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -3958,10 +4050,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>267</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -3969,7 +4061,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
         <v>28</v>
@@ -3980,18 +4072,29 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>268</v>
+      </c>
+      <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17" t="s">
         <v>51</v>
       </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
@@ -4000,144 +4103,136 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>264</v>
-      </c>
-      <c r="B19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>269</v>
       </c>
       <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" t="s">
         <v>28</v>
       </c>
-      <c r="C20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>78</v>
       </c>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
-      </c>
       <c r="C25" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>255</v>
+      </c>
+      <c r="B27" t="s">
         <v>28</v>
       </c>
-      <c r="C26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>110</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
-      </c>
       <c r="C27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
         <v>28</v>
       </c>
-      <c r="C30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>163</v>
-      </c>
-      <c r="B31" t="s">
-        <v>53</v>
-      </c>
       <c r="C31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>222</v>
+        <v>157</v>
       </c>
       <c r="B32" t="s">
-        <v>220</v>
+        <v>51</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -4145,10 +4240,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>213</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -4156,10 +4251,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>168</v>
+        <v>219</v>
       </c>
       <c r="B34" t="s">
-        <v>167</v>
+        <v>28</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -4167,10 +4262,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>162</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>161</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
@@ -4178,10 +4273,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>205</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -4189,10 +4284,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>206</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -4200,10 +4295,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -4211,10 +4306,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -4222,46 +4317,46 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" t="s">
         <v>28</v>
       </c>
-      <c r="C40" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>190</v>
-      </c>
-      <c r="B42" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" t="b">
-        <v>0</v>
-      </c>
-      <c r="D42" t="s">
-        <v>262</v>
+      <c r="C41" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -4269,12 +4364,23 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>263</v>
+        <v>187</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>252</v>
+      </c>
+      <c r="B46" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added logic for refusal
</commit_message>
<xml_diff>
--- a/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
+++ b/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A7956D-25DC-46E2-9D78-EDD7F0BE3BF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169ACD8B-BD07-4477-9EC8-AD0FC964AA84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -1269,7 +1269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
@@ -1384,8 +1384,8 @@
   <dimension ref="A1:R118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3897,9 +3897,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D46"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updates after Julie's test
</commit_message>
<xml_diff>
--- a/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
+++ b/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18AECBBC-9562-4B00-A56C-D49E5CB9D215}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5DEE76-C906-4B74-9AB8-FB527C197085}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="301">
   <si>
     <t>setting_name</t>
   </si>
@@ -410,21 +410,12 @@
     <t>data("ESTADOCRI") == "1"</t>
   </si>
   <si>
-    <t>data("BCG") == "1"</t>
-  </si>
-  <si>
     <t>Is there a reaction where the child got the BCG vaccine?</t>
   </si>
   <si>
     <t>Existe alguma reação onde a criança tomou a vacina BCG?</t>
   </si>
   <si>
-    <t>Mid-upper-arm circumference</t>
-  </si>
-  <si>
-    <t>Circunferência do meio do braço</t>
-  </si>
-  <si>
     <t>A criança recebeu BCG?</t>
   </si>
   <si>
@@ -542,12 +533,6 @@
     <t>(data("MUAC")&gt;49 &amp;&amp; data("MUAC")&lt;343 &amp;&amp; data("MUAC")%2 == 0) || data("MUAC") == 999  || data("MUAC") == "11" || data('ESTADOCRI') != 1</t>
   </si>
   <si>
-    <t>If MUAC is less than 50mm write "11" &lt;/br&gt; Ft is not possible to measure MUAC write "999"</t>
-  </si>
-  <si>
-    <t>Se o braço for menor que 50 mm, escreva "11" &lt;/br&gt; Se não for possível medir o braço, escreva "999"</t>
-  </si>
-  <si>
     <t>Must be between 50 and 342 and a even number.</t>
   </si>
   <si>
@@ -794,9 +779,6 @@
     <t>instance_name</t>
   </si>
   <si>
-    <t>data("BCGREACT") != null || data("BCG") != 1 || data('ESTADOCRI') != 1</t>
-  </si>
-  <si>
     <t>DATASAICRI</t>
   </si>
   <si>
@@ -854,12 +836,6 @@
     <t>STICKERSIMG</t>
   </si>
   <si>
-    <t>Are there any stickers on the card?</t>
-  </si>
-  <si>
-    <t>Há algum adesivo no cartão?</t>
-  </si>
-  <si>
     <t>data("STICKERS") == "1"</t>
   </si>
   <si>
@@ -882,6 +858,84 @@
   </si>
   <si>
     <t>async_assign_count</t>
+  </si>
+  <si>
+    <t>data("BCGREACT") != null || data('ESTADOCRI') != 1</t>
+  </si>
+  <si>
+    <t>data("VACINFO") == "4"</t>
+  </si>
+  <si>
+    <t>VACINFOOU</t>
+  </si>
+  <si>
+    <t>Other:</t>
+  </si>
+  <si>
+    <t>Outro:</t>
+  </si>
+  <si>
+    <t>data("VACINFOOU") != null || data("VACINFO") != 4</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Outro</t>
+  </si>
+  <si>
+    <t>OUTROVACOU</t>
+  </si>
+  <si>
+    <t>selected(data("OUTROVAC"),"Other")</t>
+  </si>
+  <si>
+    <t>Which other vaccines?</t>
+  </si>
+  <si>
+    <t>Quais outras vacinas?</t>
+  </si>
+  <si>
+    <t>data("OUTROVACOU") != null || not(selected(data("OUTROVAC"),"Other"))</t>
+  </si>
+  <si>
+    <t>Please check the child's arm for scar</t>
+  </si>
+  <si>
+    <t>Por favor, verifique se há cicatriz no braço da criança</t>
+  </si>
+  <si>
+    <t>If the child has no name write "Bebe" &lt;/br&gt; If the name is unknown write "Não sabe"</t>
+  </si>
+  <si>
+    <t>Se a criança não tiver nome escreva "Bebe" &lt;/br&gt; Se o nome for desconhecido escreva "Não sabe"</t>
+  </si>
+  <si>
+    <t>Are there any stickers or id numbers on the card?</t>
+  </si>
+  <si>
+    <t>Existe algum adesivo ou número de identificação no cartão?</t>
+  </si>
+  <si>
+    <t>Measure of the mid-upper-arm circumference</t>
+  </si>
+  <si>
+    <t>Medida da circunferência do braço</t>
+  </si>
+  <si>
+    <t>If MUAC is less than 50mm write "11" &lt;/br&gt; If it is not possible to measure MUAC write "999"</t>
+  </si>
+  <si>
+    <t>Se o MUAC for menor que 50 mm, escreva "11" &lt;/br&gt; Se não for possível medir o MUAC, escreva "999"</t>
+  </si>
+  <si>
+    <t>OBSCRI</t>
+  </si>
+  <si>
+    <t>&lt;i&gt; If you have any comment or observations about the child, write them here &lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>&lt;i&gt; Se você tiver algum comentário ou observação sobre a criança, escreva aqui &lt;/i&gt;</t>
   </si>
 </sst>
 </file>
@@ -1342,7 +1396,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1358,7 +1412,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1367,10 +1421,10 @@
       </c>
       <c r="B5" s="3"/>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1397,7 +1451,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B8" t="s">
         <v>76</v>
@@ -1414,11 +1468,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:R127"/>
+  <dimension ref="A1:R130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A106" sqref="A106:XFD106"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G129" sqref="G129:H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,7 +1550,7 @@
         <v>44</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -1509,10 +1563,10 @@
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1520,10 +1574,10 @@
         <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1531,10 +1585,10 @@
         <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H5" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1542,10 +1596,10 @@
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H6" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1553,10 +1607,10 @@
         <v>35</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1564,10 +1618,10 @@
         <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H8" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1575,10 +1629,10 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H9" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
@@ -1589,10 +1643,10 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="H10" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1610,10 +1664,10 @@
         <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H13" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1624,16 +1678,16 @@
         <v>87</v>
       </c>
       <c r="G14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="P14" t="b">
         <v>0</v>
@@ -1654,10 +1708,10 @@
         <v>35</v>
       </c>
       <c r="G17" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H17" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -1668,13 +1722,13 @@
         <v>70</v>
       </c>
       <c r="F18" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G18" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="H18" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
@@ -1685,7 +1739,7 @@
         <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
@@ -1693,16 +1747,16 @@
         <v>28</v>
       </c>
       <c r="F20" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="G20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K20" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="P20" t="b">
         <v>0</v>
@@ -1728,10 +1782,10 @@
         <v>35</v>
       </c>
       <c r="G24" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H24" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
@@ -1739,10 +1793,10 @@
         <v>35</v>
       </c>
       <c r="G25" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H25" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
@@ -1750,19 +1804,25 @@
         <v>51</v>
       </c>
       <c r="E26" t="s">
+        <v>173</v>
+      </c>
+      <c r="F26" t="s">
+        <v>177</v>
+      </c>
+      <c r="G26" t="s">
         <v>178</v>
       </c>
-      <c r="F26" t="s">
-        <v>182</v>
-      </c>
-      <c r="G26" t="s">
-        <v>183</v>
-      </c>
       <c r="H26" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="J26" t="b">
         <v>1</v>
+      </c>
+      <c r="L26" t="s">
+        <v>290</v>
+      </c>
+      <c r="M26" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
@@ -1770,7 +1830,7 @@
         <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
@@ -1810,10 +1870,10 @@
         <v>35</v>
       </c>
       <c r="G32" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H32" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
@@ -1821,10 +1881,10 @@
         <v>35</v>
       </c>
       <c r="G33" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H33" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1832,7 +1892,7 @@
         <v>68</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1840,10 +1900,10 @@
         <v>35</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I35"/>
       <c r="J35" t="b">
@@ -1860,7 +1920,7 @@
         <v>68</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1868,10 +1928,10 @@
         <v>35</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I38"/>
       <c r="J38" t="b">
@@ -1890,7 +1950,7 @@
         <v>68</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="41" spans="2:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1898,10 +1958,10 @@
         <v>35</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="I41"/>
       <c r="J41" t="b">
@@ -1918,10 +1978,10 @@
         <v>51</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
@@ -1929,7 +1989,7 @@
         <v>68</v>
       </c>
       <c r="C44" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
@@ -1972,10 +2032,10 @@
         <v>35</v>
       </c>
       <c r="G49" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H49" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.25">
@@ -1983,10 +2043,10 @@
         <v>35</v>
       </c>
       <c r="G50" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H50" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.25">
@@ -1994,16 +2054,16 @@
         <v>51</v>
       </c>
       <c r="E51" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F51" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="G51" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H51" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="J51" t="b">
         <v>1</v>
@@ -2014,7 +2074,7 @@
         <v>68</v>
       </c>
       <c r="C52" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
@@ -2034,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="K53" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="P53" t="b">
         <v>0</v>
@@ -2061,10 +2121,10 @@
         <v>35</v>
       </c>
       <c r="G57" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H57" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
@@ -2100,16 +2160,16 @@
         <v>28</v>
       </c>
       <c r="F60" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="G60" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H60" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K60" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="P60" t="b">
         <v>0</v>
@@ -2135,10 +2195,10 @@
         <v>35</v>
       </c>
       <c r="G64" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H64" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="2:16" x14ac:dyDescent="0.25">
@@ -2183,363 +2243,363 @@
     </row>
     <row r="67" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>38</v>
+        <v>68</v>
+      </c>
+      <c r="C67" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="68" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>68</v>
-      </c>
-      <c r="C68" t="s">
-        <v>117</v>
+      <c r="D68" t="s">
+        <v>61</v>
+      </c>
+      <c r="F68" t="s">
+        <v>277</v>
+      </c>
+      <c r="G68" t="s">
+        <v>278</v>
+      </c>
+      <c r="H68" t="s">
+        <v>279</v>
+      </c>
+      <c r="K68" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="69" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
-        <v>35</v>
-      </c>
-      <c r="G70" t="s">
-        <v>174</v>
-      </c>
-      <c r="H70" t="s">
-        <v>175</v>
+      <c r="B70" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="71" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>51</v>
-      </c>
-      <c r="E71" t="s">
-        <v>53</v>
-      </c>
-      <c r="F71" t="s">
-        <v>79</v>
-      </c>
-      <c r="G71" t="s">
-        <v>131</v>
-      </c>
-      <c r="H71" t="s">
-        <v>130</v>
-      </c>
-      <c r="K71" t="s">
-        <v>155</v>
+      <c r="B71" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>68</v>
-      </c>
-      <c r="C72" t="s">
-        <v>132</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
+        <v>35</v>
+      </c>
+      <c r="G73" t="s">
+        <v>169</v>
+      </c>
+      <c r="H73" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>51</v>
+      </c>
+      <c r="E74" t="s">
+        <v>53</v>
+      </c>
+      <c r="F74" t="s">
+        <v>79</v>
+      </c>
+      <c r="G74" t="s">
+        <v>128</v>
+      </c>
+      <c r="H74" t="s">
+        <v>127</v>
+      </c>
+      <c r="K74" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>68</v>
+      </c>
+      <c r="C75" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
         <v>28</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F76" t="s">
         <v>80</v>
       </c>
-      <c r="G73" t="s">
+      <c r="G76" t="s">
+        <v>130</v>
+      </c>
+      <c r="H76" t="s">
+        <v>131</v>
+      </c>
+      <c r="K76" t="s">
+        <v>153</v>
+      </c>
+      <c r="P76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>51</v>
+      </c>
+      <c r="E78" t="s">
+        <v>53</v>
+      </c>
+      <c r="F78" t="s">
+        <v>199</v>
+      </c>
+      <c r="G78" t="s">
+        <v>132</v>
+      </c>
+      <c r="H78" t="s">
         <v>133</v>
       </c>
-      <c r="H73" t="s">
-        <v>134</v>
-      </c>
-      <c r="K73" t="s">
-        <v>156</v>
-      </c>
-      <c r="P73" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>51</v>
-      </c>
-      <c r="E75" t="s">
-        <v>53</v>
-      </c>
-      <c r="F75" t="s">
-        <v>204</v>
-      </c>
-      <c r="G75" t="s">
-        <v>135</v>
-      </c>
-      <c r="H75" t="s">
-        <v>136</v>
-      </c>
-      <c r="K75" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>68</v>
-      </c>
-      <c r="C76" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
-        <v>28</v>
-      </c>
-      <c r="F77" t="s">
-        <v>205</v>
-      </c>
-      <c r="G77" t="s">
-        <v>133</v>
-      </c>
-      <c r="H77" t="s">
-        <v>134</v>
-      </c>
-      <c r="K77" t="s">
-        <v>207</v>
-      </c>
-      <c r="P77" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>69</v>
+      <c r="K78" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="79" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>28</v>
+      </c>
+      <c r="F80" t="s">
+        <v>200</v>
+      </c>
+      <c r="G80" t="s">
+        <v>130</v>
+      </c>
+      <c r="H80" t="s">
+        <v>131</v>
+      </c>
+      <c r="K80" t="s">
+        <v>202</v>
+      </c>
+      <c r="P80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D81" t="s">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
         <v>35</v>
       </c>
-      <c r="G81" t="s">
-        <v>174</v>
-      </c>
-      <c r="H81" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="82" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D82" t="s">
+      <c r="G84" t="s">
+        <v>169</v>
+      </c>
+      <c r="H84" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
         <v>51</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E85" t="s">
         <v>53</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F85" t="s">
+        <v>154</v>
+      </c>
+      <c r="G85" t="s">
+        <v>155</v>
+      </c>
+      <c r="H85" t="s">
+        <v>156</v>
+      </c>
+      <c r="K85" t="s">
         <v>157</v>
       </c>
-      <c r="G82" t="s">
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>68</v>
+      </c>
+      <c r="C87" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>35</v>
+      </c>
+      <c r="G89" t="s">
+        <v>205</v>
+      </c>
+      <c r="H89" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>207</v>
+      </c>
+      <c r="E90" t="s">
+        <v>208</v>
+      </c>
+      <c r="F90" t="s">
+        <v>209</v>
+      </c>
+      <c r="G90" t="s">
+        <v>210</v>
+      </c>
+      <c r="H90" t="s">
+        <v>211</v>
+      </c>
+      <c r="K90" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>68</v>
+      </c>
+      <c r="C91" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>61</v>
+      </c>
+      <c r="F92" t="s">
+        <v>283</v>
+      </c>
+      <c r="G92" t="s">
+        <v>285</v>
+      </c>
+      <c r="H92" t="s">
+        <v>286</v>
+      </c>
+      <c r="K92" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>28</v>
+      </c>
+      <c r="F94" t="s">
+        <v>213</v>
+      </c>
+      <c r="G94" t="s">
+        <v>214</v>
+      </c>
+      <c r="H94" t="s">
+        <v>215</v>
+      </c>
+      <c r="K94" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>35</v>
+      </c>
+      <c r="G97" t="s">
+        <v>169</v>
+      </c>
+      <c r="H97" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
         <v>158</v>
       </c>
-      <c r="H82" t="s">
+      <c r="F98" t="s">
         <v>159</v>
       </c>
-      <c r="K82" t="s">
+      <c r="G98" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="83" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="84" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>68</v>
-      </c>
-      <c r="C84" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D86" t="s">
-        <v>35</v>
-      </c>
-      <c r="G86" t="s">
-        <v>210</v>
-      </c>
-      <c r="H86" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="87" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D87" t="s">
-        <v>212</v>
-      </c>
-      <c r="E87" t="s">
-        <v>213</v>
-      </c>
-      <c r="F87" t="s">
-        <v>214</v>
-      </c>
-      <c r="G87" t="s">
-        <v>215</v>
-      </c>
-      <c r="H87" t="s">
-        <v>216</v>
-      </c>
-      <c r="K87" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="88" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D88" t="s">
-        <v>28</v>
-      </c>
-      <c r="F88" t="s">
-        <v>218</v>
-      </c>
-      <c r="G88" t="s">
-        <v>219</v>
-      </c>
-      <c r="H88" t="s">
-        <v>220</v>
-      </c>
-      <c r="K88" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="89" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="90" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>68</v>
-      </c>
-      <c r="C90" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="91" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="92" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D92" t="s">
-        <v>35</v>
-      </c>
-      <c r="G92" t="s">
-        <v>174</v>
-      </c>
-      <c r="H92" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="93" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D93" t="s">
+      <c r="H98" t="s">
         <v>161</v>
       </c>
-      <c r="F93" t="s">
+      <c r="L98" t="s">
         <v>162</v>
       </c>
-      <c r="G93" t="s">
+      <c r="M98" t="s">
         <v>163</v>
       </c>
-      <c r="H93" t="s">
+      <c r="R98" t="s">
         <v>164</v>
-      </c>
-      <c r="L93" t="s">
-        <v>165</v>
-      </c>
-      <c r="M93" t="s">
-        <v>166</v>
-      </c>
-      <c r="R93" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="94" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="95" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="96" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>68</v>
-      </c>
-      <c r="C98" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="99" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="100" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D100" t="s">
-        <v>35</v>
-      </c>
-      <c r="G100" t="s">
-        <v>174</v>
-      </c>
-      <c r="H100" t="s">
-        <v>175</v>
+      <c r="B100" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="101" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D101" t="s">
-        <v>51</v>
-      </c>
-      <c r="E101" t="s">
-        <v>53</v>
-      </c>
-      <c r="F101" t="s">
-        <v>271</v>
-      </c>
-      <c r="G101" t="s">
-        <v>273</v>
-      </c>
-      <c r="H101" t="s">
-        <v>274</v>
-      </c>
-      <c r="K101" t="s">
-        <v>279</v>
-      </c>
-      <c r="R101" t="s">
-        <v>278</v>
+      <c r="B101" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="102" spans="2:18" x14ac:dyDescent="0.25">
@@ -2547,89 +2607,83 @@
         <v>68</v>
       </c>
       <c r="C102" t="s">
-        <v>275</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D103" t="s">
-        <v>161</v>
-      </c>
-      <c r="F103" t="s">
-        <v>272</v>
-      </c>
-      <c r="G103" t="s">
-        <v>276</v>
-      </c>
-      <c r="H103" t="s">
-        <v>277</v>
+      <c r="B103" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="104" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>69</v>
+      <c r="D104" t="s">
+        <v>35</v>
+      </c>
+      <c r="G104" t="s">
+        <v>169</v>
+      </c>
+      <c r="H104" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="105" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>38</v>
+      <c r="D105" t="s">
+        <v>51</v>
+      </c>
+      <c r="E105" t="s">
+        <v>53</v>
+      </c>
+      <c r="F105" t="s">
+        <v>265</v>
+      </c>
+      <c r="G105" t="s">
+        <v>292</v>
+      </c>
+      <c r="H105" t="s">
+        <v>293</v>
+      </c>
+      <c r="K105" t="s">
+        <v>271</v>
+      </c>
+      <c r="R105" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="106" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="C106" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="107" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>68</v>
-      </c>
-      <c r="C107" t="s">
-        <v>124</v>
+      <c r="D107" t="s">
+        <v>158</v>
+      </c>
+      <c r="F107" t="s">
+        <v>266</v>
+      </c>
+      <c r="G107" t="s">
+        <v>268</v>
+      </c>
+      <c r="H107" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="108" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="109" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D109" t="s">
-        <v>35</v>
-      </c>
-      <c r="G109" t="s">
-        <v>174</v>
-      </c>
-      <c r="H109" t="s">
-        <v>175</v>
+      <c r="B109" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="110" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D110" t="s">
-        <v>49</v>
-      </c>
-      <c r="F110" t="s">
-        <v>83</v>
-      </c>
-      <c r="G110" t="s">
-        <v>128</v>
-      </c>
-      <c r="H110" t="s">
-        <v>129</v>
-      </c>
-      <c r="K110" t="s">
-        <v>168</v>
-      </c>
-      <c r="L110" t="s">
-        <v>169</v>
-      </c>
-      <c r="M110" t="s">
-        <v>170</v>
-      </c>
-      <c r="N110" t="s">
-        <v>171</v>
-      </c>
-      <c r="O110" t="s">
-        <v>172</v>
+      <c r="B110" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="111" spans="2:18" x14ac:dyDescent="0.25">
@@ -2637,143 +2691,167 @@
         <v>68</v>
       </c>
       <c r="C111" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="112" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D113" t="s">
+        <v>35</v>
+      </c>
+      <c r="G113" t="s">
+        <v>169</v>
+      </c>
+      <c r="H113" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>49</v>
+      </c>
+      <c r="F114" t="s">
+        <v>83</v>
+      </c>
+      <c r="G114" t="s">
+        <v>294</v>
+      </c>
+      <c r="H114" t="s">
+        <v>295</v>
+      </c>
+      <c r="K114" t="s">
+        <v>165</v>
+      </c>
+      <c r="L114" t="s">
+        <v>296</v>
+      </c>
+      <c r="M114" t="s">
+        <v>297</v>
+      </c>
+      <c r="N114" t="s">
+        <v>166</v>
+      </c>
+      <c r="O114" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D115" t="s">
+        <v>51</v>
+      </c>
+      <c r="E115" t="s">
+        <v>53</v>
+      </c>
+      <c r="F115" t="s">
+        <v>84</v>
+      </c>
+      <c r="G115" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="112" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D112" t="s">
-        <v>51</v>
-      </c>
-      <c r="E112" t="s">
-        <v>53</v>
-      </c>
-      <c r="F112" t="s">
-        <v>84</v>
-      </c>
-      <c r="G112" t="s">
+      <c r="H115" t="s">
         <v>126</v>
       </c>
-      <c r="H112" t="s">
-        <v>127</v>
-      </c>
-      <c r="K112" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>69</v>
+      <c r="K115" t="s">
+        <v>275</v>
+      </c>
+      <c r="L115" t="s">
+        <v>288</v>
+      </c>
+      <c r="M115" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="116" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D117" t="s">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
         <v>35</v>
       </c>
-      <c r="G117" t="s">
-        <v>174</v>
-      </c>
-      <c r="H117" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D118" t="s">
-        <v>51</v>
-      </c>
-      <c r="E118" t="s">
-        <v>54</v>
-      </c>
-      <c r="F118" t="s">
-        <v>85</v>
-      </c>
-      <c r="G118" t="s">
-        <v>137</v>
-      </c>
-      <c r="H118" t="s">
-        <v>141</v>
-      </c>
-      <c r="J118" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
-        <v>68</v>
-      </c>
-      <c r="C119" t="s">
-        <v>138</v>
+      <c r="G119" t="s">
+        <v>169</v>
+      </c>
+      <c r="H119" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="120" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D120" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="E120" t="s">
+        <v>54</v>
       </c>
       <c r="F120" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G120" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H120" t="s">
-        <v>140</v>
-      </c>
-      <c r="K120" t="s">
-        <v>173</v>
-      </c>
-      <c r="P120" t="b">
-        <v>0</v>
+        <v>138</v>
+      </c>
+      <c r="J120" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="C121" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="122" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B122" t="s">
-        <v>38</v>
+      <c r="D122" t="s">
+        <v>28</v>
+      </c>
+      <c r="F122" t="s">
+        <v>86</v>
+      </c>
+      <c r="G122" t="s">
+        <v>136</v>
+      </c>
+      <c r="H122" t="s">
+        <v>137</v>
+      </c>
+      <c r="K122" t="s">
+        <v>168</v>
+      </c>
+      <c r="P122" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D124" t="s">
-        <v>35</v>
-      </c>
-      <c r="G124" t="s">
-        <v>174</v>
-      </c>
-      <c r="H124" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D125" t="s">
-        <v>35</v>
-      </c>
-      <c r="G125" t="s">
-        <v>236</v>
-      </c>
-      <c r="H125" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="126" spans="2:16" x14ac:dyDescent="0.25">
@@ -2781,14 +2859,50 @@
         <v>35</v>
       </c>
       <c r="G126" t="s">
-        <v>238</v>
+        <v>169</v>
       </c>
       <c r="H126" t="s">
-        <v>239</v>
+        <v>170</v>
       </c>
     </row>
     <row r="127" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B127" t="s">
+      <c r="D127" t="s">
+        <v>35</v>
+      </c>
+      <c r="G127" t="s">
+        <v>231</v>
+      </c>
+      <c r="H127" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D128" t="s">
+        <v>35</v>
+      </c>
+      <c r="G128" t="s">
+        <v>233</v>
+      </c>
+      <c r="H128" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D129" t="s">
+        <v>61</v>
+      </c>
+      <c r="F129" t="s">
+        <v>298</v>
+      </c>
+      <c r="G129" t="s">
+        <v>299</v>
+      </c>
+      <c r="H129" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2800,11 +2914,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:F146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2831,32 +2945,32 @@
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B2" s="11" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B3" s="11" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -3196,86 +3310,95 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
+      <c r="A30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>281</v>
+      </c>
+      <c r="D30" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>213</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>208</v>
+      </c>
+      <c r="B32" t="s">
+        <v>217</v>
+      </c>
+      <c r="C32" t="s">
+        <v>218</v>
+      </c>
+      <c r="D32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>208</v>
+      </c>
+      <c r="B33" t="s">
+        <v>220</v>
+      </c>
+      <c r="C33" t="s">
+        <v>221</v>
+      </c>
+      <c r="D33" t="s">
         <v>222</v>
-      </c>
-      <c r="C31" t="s">
-        <v>223</v>
-      </c>
-      <c r="D31" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>213</v>
-      </c>
-      <c r="B32" t="s">
-        <v>225</v>
-      </c>
-      <c r="C32" t="s">
-        <v>226</v>
-      </c>
-      <c r="D32" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>213</v>
-      </c>
-      <c r="B33" t="s">
-        <v>228</v>
-      </c>
-      <c r="C33" t="s">
-        <v>229</v>
-      </c>
-      <c r="D33" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B34" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="C34" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D34" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B35" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C35" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D35" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
+      <c r="A36" t="s">
+        <v>208</v>
+      </c>
+      <c r="B36" t="s">
+        <v>229</v>
+      </c>
+      <c r="C36" t="s">
+        <v>229</v>
+      </c>
+      <c r="D36" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
@@ -3284,16 +3407,16 @@
       <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
@@ -3307,28 +3430,28 @@
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="16"/>
+      <c r="D42" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="F43" s="13"/>
+      <c r="D43" s="16"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
+      <c r="F44" s="13"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
-      <c r="B45" s="11"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
     </row>
@@ -3352,17 +3475,17 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
+      <c r="B49" s="11"/>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-    </row>
-    <row r="51" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -3376,7 +3499,7 @@
     </row>
     <row r="53" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13"/>
-      <c r="B53" s="11"/>
+      <c r="B53" s="13"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
     </row>
@@ -3387,16 +3510,16 @@
       <c r="D54" s="13"/>
     </row>
     <row r="55" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
+      <c r="A55" s="13"/>
       <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+    </row>
+    <row r="56" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="13"/>
@@ -3411,13 +3534,13 @@
       <c r="D58" s="14"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
+      <c r="A60" s="14"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
@@ -3448,7 +3571,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
-      <c r="B65" s="17"/>
+      <c r="B65" s="13"/>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
     </row>
@@ -3460,9 +3583,9 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="19"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
@@ -3592,9 +3715,9 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="19"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="13"/>
@@ -3605,14 +3728,14 @@
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
       <c r="B91" s="17"/>
-      <c r="C91" s="19"/>
-      <c r="D91" s="19"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
       <c r="B92" s="17"/>
       <c r="C92" s="19"/>
-      <c r="D92" s="14"/>
+      <c r="D92" s="19"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
@@ -3623,7 +3746,7 @@
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
       <c r="B94" s="17"/>
-      <c r="C94" s="15"/>
+      <c r="C94" s="19"/>
       <c r="D94" s="14"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3635,13 +3758,13 @@
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="13"/>
       <c r="B96" s="17"/>
-      <c r="C96" s="14"/>
+      <c r="C96" s="15"/>
       <c r="D96" s="14"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
       <c r="B97" s="17"/>
-      <c r="C97" s="15"/>
+      <c r="C97" s="14"/>
       <c r="D97" s="14"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3676,7 +3799,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="13"/>
-      <c r="B103" s="13"/>
+      <c r="B103" s="17"/>
       <c r="C103" s="15"/>
       <c r="D103" s="14"/>
     </row>
@@ -3700,7 +3823,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
-      <c r="B107" s="17"/>
+      <c r="B107" s="13"/>
       <c r="C107" s="15"/>
       <c r="D107" s="14"/>
     </row>
@@ -3712,7 +3835,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="13"/>
-      <c r="B109" s="13"/>
+      <c r="B109" s="17"/>
       <c r="C109" s="15"/>
       <c r="D109" s="14"/>
     </row>
@@ -3724,13 +3847,13 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="13"/>
-      <c r="B111" s="17"/>
+      <c r="B111" s="13"/>
       <c r="C111" s="15"/>
       <c r="D111" s="14"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="13"/>
-      <c r="B112" s="13"/>
+      <c r="B112" s="17"/>
       <c r="C112" s="15"/>
       <c r="D112" s="14"/>
     </row>
@@ -3748,13 +3871,13 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="13"/>
-      <c r="B115" s="17"/>
+      <c r="B115" s="13"/>
       <c r="C115" s="15"/>
       <c r="D115" s="14"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="13"/>
-      <c r="B116" s="13"/>
+      <c r="B116" s="17"/>
       <c r="C116" s="15"/>
       <c r="D116" s="14"/>
     </row>
@@ -3767,18 +3890,18 @@
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="13"/>
       <c r="B118" s="13"/>
-      <c r="C118" s="14"/>
+      <c r="C118" s="15"/>
       <c r="D118" s="14"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="13"/>
-      <c r="B119" s="17"/>
-      <c r="C119" s="15"/>
+      <c r="B119" s="13"/>
+      <c r="C119" s="14"/>
       <c r="D119" s="14"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="13"/>
-      <c r="B120" s="13"/>
+      <c r="B120" s="17"/>
       <c r="C120" s="15"/>
       <c r="D120" s="14"/>
     </row>
@@ -3802,13 +3925,13 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="13"/>
-      <c r="B124" s="17"/>
+      <c r="B124" s="13"/>
       <c r="C124" s="15"/>
       <c r="D124" s="14"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="13"/>
-      <c r="B125" s="13"/>
+      <c r="B125" s="17"/>
       <c r="C125" s="15"/>
       <c r="D125" s="14"/>
     </row>
@@ -3821,7 +3944,7 @@
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="13"/>
       <c r="B127" s="13"/>
-      <c r="C127" s="14"/>
+      <c r="C127" s="15"/>
       <c r="D127" s="14"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -3832,20 +3955,21 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="13"/>
-      <c r="B129" s="17"/>
+      <c r="B129" s="13"/>
       <c r="C129" s="14"/>
       <c r="D129" s="14"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B130" s="6"/>
+      <c r="A130" s="13"/>
+      <c r="B130" s="17"/>
+      <c r="C130" s="14"/>
+      <c r="D130" s="14"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B131" s="6"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="6"/>
-      <c r="C132"/>
-      <c r="D132"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
@@ -3911,6 +4035,11 @@
       <c r="B145" s="6"/>
       <c r="C145"/>
       <c r="D145"/>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146" s="6"/>
+      <c r="C146"/>
+      <c r="D146"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -3944,10 +4073,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -4009,11 +4138,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4049,7 +4178,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -4142,7 +4271,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
@@ -4153,7 +4282,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B12" t="s">
         <v>61</v>
@@ -4164,7 +4293,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B14" t="s">
         <v>61</v>
@@ -4186,7 +4315,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B16" t="s">
         <v>61</v>
@@ -4197,7 +4326,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B17" t="s">
         <v>51</v>
@@ -4208,7 +4337,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
@@ -4219,7 +4348,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B20" t="s">
         <v>61</v>
@@ -4230,7 +4359,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B21" t="s">
         <v>51</v>
@@ -4241,16 +4370,16 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B23" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C23" t="b">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4310,7 +4439,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
@@ -4343,95 +4472,95 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>277</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>79</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>51</v>
       </c>
-      <c r="C32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>80</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>28</v>
       </c>
-      <c r="C33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>157</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" t="s">
         <v>51</v>
       </c>
-      <c r="C34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>214</v>
-      </c>
-      <c r="B35" t="s">
-        <v>212</v>
-      </c>
       <c r="C35" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B36" t="s">
+        <v>207</v>
+      </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>283</v>
+      </c>
+      <c r="B37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>213</v>
+      </c>
+      <c r="B38" t="s">
         <v>28</v>
       </c>
-      <c r="C36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>162</v>
-      </c>
-      <c r="B37" t="s">
-        <v>161</v>
-      </c>
-      <c r="C37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>271</v>
-      </c>
-      <c r="B38" t="s">
-        <v>51</v>
-      </c>
       <c r="C38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>272</v>
+        <v>159</v>
       </c>
       <c r="B39" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>204</v>
+        <v>265</v>
       </c>
       <c r="B40" t="s">
         <v>51</v>
@@ -4440,105 +4569,138 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>205</v>
+        <v>266</v>
       </c>
       <c r="B41" t="s">
+        <v>158</v>
+      </c>
+      <c r="C41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>200</v>
+      </c>
+      <c r="B43" t="s">
         <v>28</v>
       </c>
-      <c r="C41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>83</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" t="s">
         <v>49</v>
       </c>
-      <c r="C42" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>84</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B45" t="s">
         <v>51</v>
       </c>
-      <c r="C43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>85</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>51</v>
       </c>
-      <c r="C44" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>86</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>28</v>
       </c>
-      <c r="C45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>182</v>
-      </c>
-      <c r="B47" t="s">
-        <v>51</v>
-      </c>
       <c r="C47" t="b">
         <v>0</v>
       </c>
-      <c r="D47" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>185</v>
+        <v>298</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>186</v>
-      </c>
-      <c r="B49" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>251</v>
+        <v>177</v>
       </c>
       <c r="B50" t="s">
         <v>51</v>
       </c>
       <c r="C50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>181</v>
+      </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>246</v>
+      </c>
+      <c r="B53" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to list and children
</commit_message>
<xml_diff>
--- a/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
+++ b/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAE9A1E-58F1-477F-952A-B7D099ED8EBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0CD5AA-91DC-4E60-AEB0-52B5F52DFA14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="335">
   <si>
     <t>setting_name</t>
   </si>
@@ -852,12 +852,6 @@
   </si>
   <si>
     <t>data("OUTROVACOU") != null || not(selected(data("OUTROVAC"),"Other"))</t>
-  </si>
-  <si>
-    <t>Please check the child's arm for scar</t>
-  </si>
-  <si>
-    <t>Por favor, verifique se há cicatriz no braço da criança</t>
   </si>
   <si>
     <t>If the child has no name write "Bebe" &lt;/br&gt; If the name is unknown write "Não sabe"</t>
@@ -967,6 +961,84 @@
   </si>
   <si>
     <t>muac.jpg</t>
+  </si>
+  <si>
+    <t>bcgpolio</t>
+  </si>
+  <si>
+    <t>data("bcgcheck") == "1"</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>data("poliocheck") == "1"</t>
+  </si>
+  <si>
+    <t>data("bcgcheck") != "2" &amp;&amp; not(adate.diffInDays(data("BCGDATA"),data("DATASEG")) &gt;= 0 &amp;&amp; adate.diffInDays(data("REGDIA"),data("BCGDATA")) &gt;= 0 &amp;&amp; data("BCGDATA") != null &amp;&amp; adate.ageInYears(data("BCGDATA")) != -9999 &amp;&amp; adate.ageInYears(data("BCGDATA")) &lt; 2019) &amp;&amp; data("BCG") == 1</t>
+  </si>
+  <si>
+    <t>obsbcg</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Follow-up on registered pregnancy to {{data.NOMEMUL}} regdia: {{calculates.displayREGDIA}}&lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Seguimento de gravidez registrada para {{data.NOMEMUL}} regdia: {{calculates.displayREGDIA}} &lt;/b&gt;</t>
+  </si>
+  <si>
+    <t>&lt;font color = "red"&gt; Date of BCG vaccination is after today or before birth. &lt;/br&gt; Please check vaccine again. &lt;/font&gt;</t>
+  </si>
+  <si>
+    <t>&lt;font color = "red"&gt; A data da vacinação BCG é depois de hoje ou antes do nascimento. &lt;/br&gt; Por favor, verifique a vacina novamente. &lt;/font&gt;</t>
+  </si>
+  <si>
+    <t>data("poliocheck") != "2" &amp;&amp; not(adate.diffInDays(data("POLIODATA"),data("DATASEG")) &gt;= 0 &amp;&amp; adate.diffInDays(data("REGDIA"),data("POLIODATA")) &gt;= 0 &amp;&amp; data("POLIODATA") != null &amp;&amp; adate.ageInYears(data("POLIODATA")) != -9999 &amp;&amp; adate.ageInYears(data("POLIODATA")) &lt; 2019) &amp;&amp; data("POLIO") == 1</t>
+  </si>
+  <si>
+    <t>obspolio</t>
+  </si>
+  <si>
+    <t>&lt;font color = "red"&gt; Date of polio vaccination is after today or before birth. &lt;/br&gt; Please check vaccine again. &lt;/font&gt;</t>
+  </si>
+  <si>
+    <t>&lt;font color = "red"&gt; A data da vacinação contra polio (VPO-0) é depois de hoje ou antes do nascimento. &lt;/br&gt; Por favor, verifique a vacina novamente. &lt;/font&gt;</t>
+  </si>
+  <si>
+    <t>data("bcgcheck") == "1" || data("poliocheck") == "1"</t>
+  </si>
+  <si>
+    <t>goto bcgpolio</t>
+  </si>
+  <si>
+    <t>outrovac</t>
+  </si>
+  <si>
+    <t>data("outrocheck") == "1"</t>
+  </si>
+  <si>
+    <t>outrocheck</t>
+  </si>
+  <si>
+    <t>data("outrocheck") != "2" &amp;&amp; not(adate.diffInDays(data("OUTRODATA"),data("DATASEG")) &gt;= 0 &amp;&amp; adate.diffInDays(data("REGDIA"),data("OUTRODATA")) &gt;= 0 &amp;&amp; data("OUTRODATA") != null &amp;&amp; adate.ageInYears(data("OUTRODATA")) != -9999 &amp;&amp; adate.ageInYears(data("OUTRODATA")) &lt; 2019) &amp;&amp; data("VACINASOU") == 1</t>
+  </si>
+  <si>
+    <t>obsoutro</t>
+  </si>
+  <si>
+    <t>&lt;font color = "red"&gt; Date of first vaccination is after today or before birth. &lt;/br&gt; Please check vaccine again. &lt;/font&gt;</t>
+  </si>
+  <si>
+    <t>&lt;font color = "red"&gt; A data da primeira vacina é depois de hoje ou antes do nascimento. &lt;/br&gt; Por favor, verifique a vacina novamente. &lt;/font&gt;</t>
+  </si>
+  <si>
+    <t>goto outrovac</t>
+  </si>
+  <si>
+    <t>Please check the child's arm for a reaction</t>
+  </si>
+  <si>
+    <t>Por favor, verifique o braço da criança para ver uma reação</t>
   </si>
 </sst>
 </file>
@@ -1493,11 +1565,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:R132"/>
+  <dimension ref="A1:R170"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J156" sqref="J156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,10 +1660,10 @@
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1678,10 +1750,10 @@
         <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H12" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1722,10 +1794,10 @@
         <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H16" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
@@ -1770,13 +1842,13 @@
         <v>146</v>
       </c>
       <c r="K19" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="N19" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="O19" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="P19" t="b">
         <v>0</v>
@@ -1802,10 +1874,10 @@
         <v>35</v>
       </c>
       <c r="G23" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H23" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
@@ -1839,10 +1911,10 @@
         <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="M25" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
@@ -1867,7 +1939,7 @@
         <v>87</v>
       </c>
       <c r="K27" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
@@ -1890,10 +1962,10 @@
         <v>35</v>
       </c>
       <c r="G31" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H31" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
@@ -2029,7 +2101,7 @@
         <v>90</v>
       </c>
       <c r="K44" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
@@ -2052,10 +2124,10 @@
         <v>35</v>
       </c>
       <c r="G48" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H48" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.25">
@@ -2111,13 +2183,13 @@
         <v>92</v>
       </c>
       <c r="K52" t="s">
+        <v>291</v>
+      </c>
+      <c r="N52" t="s">
+        <v>292</v>
+      </c>
+      <c r="O52" t="s">
         <v>293</v>
-      </c>
-      <c r="N52" t="s">
-        <v>294</v>
-      </c>
-      <c r="O52" t="s">
-        <v>295</v>
       </c>
       <c r="P52" t="b">
         <v>0</v>
@@ -2144,10 +2216,10 @@
         <v>35</v>
       </c>
       <c r="G56" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H56" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.25">
@@ -2192,13 +2264,13 @@
         <v>146</v>
       </c>
       <c r="K59" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="N59" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="O59" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="P59" t="b">
         <v>0</v>
@@ -2224,10 +2296,10 @@
         <v>35</v>
       </c>
       <c r="G63" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H63" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.25">
@@ -2250,7 +2322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>50</v>
       </c>
@@ -2270,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>67</v>
       </c>
@@ -2278,7 +2350,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>60</v>
       </c>
@@ -2295,17 +2367,17 @@
         <v>265</v>
       </c>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>67</v>
       </c>
@@ -2313,23 +2385,26 @@
         <v>115</v>
       </c>
     </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>309</v>
+      </c>
       <c r="B71" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>35</v>
       </c>
       <c r="G72" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="H72" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
         <v>50</v>
       </c>
@@ -2349,7 +2424,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>67</v>
       </c>
@@ -2357,7 +2432,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>28</v>
       </c>
@@ -2377,12 +2452,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
         <v>50</v>
       </c>
@@ -2402,7 +2477,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>67</v>
       </c>
@@ -2410,7 +2485,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
         <v>28</v>
       </c>
@@ -2430,550 +2505,860 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
+        <v>67</v>
+      </c>
+      <c r="C81" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>311</v>
+      </c>
+      <c r="F82" t="s">
+        <v>302</v>
+      </c>
+      <c r="I82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>68</v>
+      </c>
+      <c r="I83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>67</v>
+      </c>
+      <c r="C84" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>311</v>
+      </c>
+      <c r="F85" t="s">
+        <v>303</v>
+      </c>
+      <c r="I85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>68</v>
+      </c>
+      <c r="I86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>67</v>
+      </c>
+      <c r="C88" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>314</v>
+      </c>
+      <c r="B89" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D83" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
         <v>35</v>
       </c>
-      <c r="G83" t="s">
-        <v>296</v>
-      </c>
-      <c r="H83" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D84" t="s">
+      <c r="G90" t="s">
+        <v>294</v>
+      </c>
+      <c r="H90" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>35</v>
+      </c>
+      <c r="G91" t="s">
+        <v>317</v>
+      </c>
+      <c r="H91" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D92" t="s">
+        <v>311</v>
+      </c>
+      <c r="F92" t="s">
+        <v>302</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>67</v>
+      </c>
+      <c r="C95" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>320</v>
+      </c>
+      <c r="B96" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D97" t="s">
+        <v>35</v>
+      </c>
+      <c r="G97" t="s">
+        <v>294</v>
+      </c>
+      <c r="H97" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D98" t="s">
+        <v>35</v>
+      </c>
+      <c r="G98" t="s">
+        <v>321</v>
+      </c>
+      <c r="H98" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D99" t="s">
+        <v>311</v>
+      </c>
+      <c r="F99" t="s">
+        <v>303</v>
+      </c>
+      <c r="I99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>67</v>
+      </c>
+      <c r="C102" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D106" t="s">
+        <v>35</v>
+      </c>
+      <c r="G106" t="s">
+        <v>294</v>
+      </c>
+      <c r="H106" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D107" t="s">
         <v>50</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E107" t="s">
         <v>52</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F107" t="s">
         <v>149</v>
       </c>
-      <c r="G84" t="s">
+      <c r="G107" t="s">
         <v>150</v>
       </c>
-      <c r="H84" t="s">
+      <c r="H107" t="s">
         <v>151</v>
       </c>
-      <c r="K84" t="s">
+      <c r="K107" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>67</v>
-      </c>
-      <c r="C86" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="87" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D88" t="s">
-        <v>35</v>
-      </c>
-      <c r="G88" t="s">
-        <v>296</v>
-      </c>
-      <c r="H88" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D89" t="s">
-        <v>197</v>
-      </c>
-      <c r="E89" t="s">
-        <v>198</v>
-      </c>
-      <c r="F89" t="s">
-        <v>199</v>
-      </c>
-      <c r="G89" t="s">
-        <v>200</v>
-      </c>
-      <c r="H89" t="s">
-        <v>201</v>
-      </c>
-      <c r="K89" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>67</v>
-      </c>
-      <c r="C90" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D91" t="s">
-        <v>60</v>
-      </c>
-      <c r="F91" t="s">
-        <v>268</v>
-      </c>
-      <c r="G91" t="s">
-        <v>270</v>
-      </c>
-      <c r="H91" t="s">
-        <v>271</v>
-      </c>
-      <c r="K91" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D93" t="s">
-        <v>28</v>
-      </c>
-      <c r="F93" t="s">
-        <v>203</v>
-      </c>
-      <c r="G93" t="s">
-        <v>204</v>
-      </c>
-      <c r="H93" t="s">
-        <v>205</v>
-      </c>
-      <c r="K93" t="s">
-        <v>286</v>
-      </c>
-      <c r="P93" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D96" t="s">
-        <v>35</v>
-      </c>
-      <c r="G96" t="s">
-        <v>296</v>
-      </c>
-      <c r="H96" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D97" t="s">
-        <v>153</v>
-      </c>
-      <c r="F97" t="s">
-        <v>154</v>
-      </c>
-      <c r="G97" t="s">
-        <v>155</v>
-      </c>
-      <c r="H97" t="s">
-        <v>156</v>
-      </c>
-      <c r="L97" t="s">
-        <v>157</v>
-      </c>
-      <c r="M97" t="s">
-        <v>158</v>
-      </c>
-      <c r="R97" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="99" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="100" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="101" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>67</v>
-      </c>
-      <c r="C101" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="102" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="103" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D103" t="s">
-        <v>35</v>
-      </c>
-      <c r="G103" t="s">
-        <v>296</v>
-      </c>
-      <c r="H103" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="104" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D104" t="s">
-        <v>50</v>
-      </c>
-      <c r="E104" t="s">
-        <v>52</v>
-      </c>
-      <c r="F104" t="s">
-        <v>250</v>
-      </c>
-      <c r="G104" t="s">
-        <v>277</v>
-      </c>
-      <c r="H104" t="s">
-        <v>278</v>
-      </c>
-      <c r="K104" t="s">
-        <v>256</v>
-      </c>
-      <c r="R104" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="105" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>67</v>
-      </c>
-      <c r="C105" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="106" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D106" t="s">
-        <v>153</v>
-      </c>
-      <c r="F106" t="s">
-        <v>251</v>
-      </c>
-      <c r="G106" t="s">
-        <v>253</v>
-      </c>
-      <c r="H106" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="107" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="108" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
+        <v>67</v>
+      </c>
+      <c r="C109" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>325</v>
+      </c>
+      <c r="B110" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D111" t="s">
+        <v>35</v>
+      </c>
+      <c r="G111" t="s">
+        <v>294</v>
+      </c>
+      <c r="H111" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D112" t="s">
+        <v>197</v>
+      </c>
+      <c r="E112" t="s">
+        <v>198</v>
+      </c>
+      <c r="F112" t="s">
+        <v>199</v>
+      </c>
+      <c r="G112" t="s">
+        <v>200</v>
+      </c>
+      <c r="H112" t="s">
+        <v>201</v>
+      </c>
+      <c r="K112" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>67</v>
+      </c>
+      <c r="C113" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D114" t="s">
+        <v>60</v>
+      </c>
+      <c r="F114" t="s">
+        <v>268</v>
+      </c>
+      <c r="G114" t="s">
+        <v>270</v>
+      </c>
+      <c r="H114" t="s">
+        <v>271</v>
+      </c>
+      <c r="K114" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="110" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D116" t="s">
+        <v>28</v>
+      </c>
+      <c r="F116" t="s">
+        <v>203</v>
+      </c>
+      <c r="G116" t="s">
+        <v>204</v>
+      </c>
+      <c r="H116" t="s">
+        <v>205</v>
+      </c>
+      <c r="K116" t="s">
+        <v>284</v>
+      </c>
+      <c r="P116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
         <v>67</v>
       </c>
-      <c r="C110" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="111" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="112" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D112" t="s">
-        <v>35</v>
-      </c>
-      <c r="G112" t="s">
-        <v>296</v>
-      </c>
-      <c r="H112" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="113" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D113" t="s">
-        <v>48</v>
-      </c>
-      <c r="F113" t="s">
-        <v>81</v>
-      </c>
-      <c r="G113" t="s">
-        <v>279</v>
-      </c>
-      <c r="H113" t="s">
-        <v>280</v>
-      </c>
-      <c r="K113" t="s">
-        <v>160</v>
-      </c>
-      <c r="L113" t="s">
-        <v>281</v>
-      </c>
-      <c r="M113" t="s">
-        <v>282</v>
-      </c>
-      <c r="N113" t="s">
-        <v>161</v>
-      </c>
-      <c r="O113" t="s">
-        <v>162</v>
-      </c>
-      <c r="R113" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="114" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="115" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="116" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D116" t="s">
-        <v>35</v>
-      </c>
-      <c r="G116" t="s">
-        <v>296</v>
-      </c>
-      <c r="H116" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="117" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D117" t="s">
-        <v>50</v>
-      </c>
-      <c r="E117" t="s">
-        <v>52</v>
-      </c>
-      <c r="F117" t="s">
-        <v>82</v>
-      </c>
-      <c r="G117" t="s">
-        <v>123</v>
-      </c>
-      <c r="H117" t="s">
-        <v>124</v>
-      </c>
-      <c r="K117" t="s">
-        <v>260</v>
-      </c>
-      <c r="L117" t="s">
-        <v>273</v>
-      </c>
-      <c r="M117" t="s">
-        <v>274</v>
-      </c>
-      <c r="R117" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="118" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B118" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="119" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D118" t="s">
+        <v>311</v>
+      </c>
+      <c r="F118" t="s">
+        <v>327</v>
+      </c>
+      <c r="I118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="120" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="I119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>67</v>
+      </c>
+      <c r="C121" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>329</v>
+      </c>
+      <c r="B122" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="121" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D121" t="s">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
         <v>35</v>
       </c>
-      <c r="G121" t="s">
-        <v>296</v>
-      </c>
-      <c r="H121" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="122" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D122" t="s">
-        <v>50</v>
-      </c>
-      <c r="E122" t="s">
-        <v>53</v>
-      </c>
-      <c r="F122" t="s">
-        <v>83</v>
-      </c>
-      <c r="G122" t="s">
-        <v>302</v>
-      </c>
-      <c r="H122" t="s">
-        <v>303</v>
-      </c>
-      <c r="J122" t="b">
+      <c r="G123" t="s">
+        <v>315</v>
+      </c>
+      <c r="H123" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D124" t="s">
+        <v>35</v>
+      </c>
+      <c r="G124" t="s">
+        <v>330</v>
+      </c>
+      <c r="H124" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D125" t="s">
+        <v>311</v>
+      </c>
+      <c r="F125" t="s">
+        <v>327</v>
+      </c>
+      <c r="I125">
         <v>1</v>
       </c>
-      <c r="L122" t="s">
-        <v>288</v>
-      </c>
-      <c r="M122" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="123" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
-        <v>67</v>
-      </c>
-      <c r="C123" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="124" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D124" t="s">
-        <v>28</v>
-      </c>
-      <c r="F124" t="s">
-        <v>84</v>
-      </c>
-      <c r="G124" t="s">
-        <v>133</v>
-      </c>
-      <c r="H124" t="s">
-        <v>134</v>
-      </c>
-      <c r="K124" s="20" t="s">
-        <v>308</v>
-      </c>
-      <c r="N124" t="s">
-        <v>300</v>
-      </c>
-      <c r="O124" t="s">
-        <v>301</v>
-      </c>
-      <c r="P124" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B125" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="126" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="127" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>67</v>
+      </c>
+      <c r="C128" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="129" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="130" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="131" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="132" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="133" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>67</v>
+      </c>
+      <c r="C133" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="134" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>67</v>
+      </c>
+      <c r="C134" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="135" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="128" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="D128" t="s">
+    <row r="136" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D136" t="s">
         <v>35</v>
       </c>
-      <c r="G128" t="s">
-        <v>296</v>
-      </c>
-      <c r="H128" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D129" t="s">
+      <c r="G136" t="s">
+        <v>294</v>
+      </c>
+      <c r="H136" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="137" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
+        <v>153</v>
+      </c>
+      <c r="F137" t="s">
+        <v>154</v>
+      </c>
+      <c r="G137" t="s">
+        <v>155</v>
+      </c>
+      <c r="H137" t="s">
+        <v>156</v>
+      </c>
+      <c r="L137" t="s">
+        <v>157</v>
+      </c>
+      <c r="M137" t="s">
+        <v>158</v>
+      </c>
+      <c r="R137" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="138" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="139" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="140" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="141" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D141" t="s">
         <v>35</v>
       </c>
-      <c r="G129" t="s">
+      <c r="G141" t="s">
+        <v>294</v>
+      </c>
+      <c r="H141" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="142" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D142" t="s">
+        <v>50</v>
+      </c>
+      <c r="E142" t="s">
+        <v>52</v>
+      </c>
+      <c r="F142" t="s">
+        <v>250</v>
+      </c>
+      <c r="G142" t="s">
+        <v>275</v>
+      </c>
+      <c r="H142" t="s">
+        <v>276</v>
+      </c>
+      <c r="K142" t="s">
+        <v>256</v>
+      </c>
+      <c r="R142" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="143" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>67</v>
+      </c>
+      <c r="C143" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="144" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D144" t="s">
+        <v>153</v>
+      </c>
+      <c r="F144" t="s">
+        <v>251</v>
+      </c>
+      <c r="G144" t="s">
+        <v>253</v>
+      </c>
+      <c r="H144" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="145" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="146" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="147" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="148" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>67</v>
+      </c>
+      <c r="C148" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="149" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="150" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D150" t="s">
+        <v>35</v>
+      </c>
+      <c r="G150" t="s">
+        <v>294</v>
+      </c>
+      <c r="H150" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="151" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D151" t="s">
+        <v>48</v>
+      </c>
+      <c r="F151" t="s">
+        <v>81</v>
+      </c>
+      <c r="G151" t="s">
+        <v>277</v>
+      </c>
+      <c r="H151" t="s">
+        <v>278</v>
+      </c>
+      <c r="K151" t="s">
+        <v>160</v>
+      </c>
+      <c r="L151" t="s">
+        <v>279</v>
+      </c>
+      <c r="M151" t="s">
+        <v>280</v>
+      </c>
+      <c r="N151" t="s">
+        <v>161</v>
+      </c>
+      <c r="O151" t="s">
+        <v>162</v>
+      </c>
+      <c r="R151" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="152" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="153" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="154" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D154" t="s">
+        <v>35</v>
+      </c>
+      <c r="G154" t="s">
+        <v>294</v>
+      </c>
+      <c r="H154" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="155" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
+        <v>50</v>
+      </c>
+      <c r="E155" t="s">
+        <v>52</v>
+      </c>
+      <c r="F155" t="s">
+        <v>82</v>
+      </c>
+      <c r="G155" t="s">
+        <v>123</v>
+      </c>
+      <c r="H155" t="s">
+        <v>124</v>
+      </c>
+      <c r="K155" t="s">
+        <v>260</v>
+      </c>
+      <c r="L155" t="s">
+        <v>333</v>
+      </c>
+      <c r="M155" t="s">
+        <v>334</v>
+      </c>
+      <c r="R155" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="156" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="157" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="158" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="159" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D159" t="s">
+        <v>35</v>
+      </c>
+      <c r="G159" t="s">
+        <v>294</v>
+      </c>
+      <c r="H159" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="160" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D160" t="s">
+        <v>50</v>
+      </c>
+      <c r="E160" t="s">
+        <v>53</v>
+      </c>
+      <c r="F160" t="s">
+        <v>83</v>
+      </c>
+      <c r="G160" t="s">
+        <v>300</v>
+      </c>
+      <c r="H160" t="s">
+        <v>301</v>
+      </c>
+      <c r="J160" t="b">
+        <v>1</v>
+      </c>
+      <c r="L160" t="s">
+        <v>286</v>
+      </c>
+      <c r="M160" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="161" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>67</v>
+      </c>
+      <c r="C161" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="162" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D162" t="s">
+        <v>28</v>
+      </c>
+      <c r="F162" t="s">
+        <v>84</v>
+      </c>
+      <c r="G162" t="s">
+        <v>133</v>
+      </c>
+      <c r="H162" t="s">
+        <v>134</v>
+      </c>
+      <c r="K162" s="20" t="s">
+        <v>306</v>
+      </c>
+      <c r="N162" t="s">
+        <v>298</v>
+      </c>
+      <c r="O162" t="s">
+        <v>299</v>
+      </c>
+      <c r="P162" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="164" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="165" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="166" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D166" t="s">
+        <v>35</v>
+      </c>
+      <c r="G166" t="s">
+        <v>294</v>
+      </c>
+      <c r="H166" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="167" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D167" t="s">
+        <v>35</v>
+      </c>
+      <c r="G167" t="s">
         <v>220</v>
       </c>
-      <c r="H129" t="s">
+      <c r="H167" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D130" t="s">
+    <row r="168" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D168" t="s">
         <v>35</v>
       </c>
-      <c r="G130" t="s">
+      <c r="G168" t="s">
         <v>222</v>
       </c>
-      <c r="H130" t="s">
+      <c r="H168" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D131" t="s">
+    <row r="169" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D169" t="s">
         <v>60</v>
       </c>
-      <c r="F131" t="s">
+      <c r="F169" t="s">
+        <v>281</v>
+      </c>
+      <c r="G169" t="s">
+        <v>282</v>
+      </c>
+      <c r="H169" t="s">
         <v>283</v>
       </c>
-      <c r="G131" t="s">
-        <v>284</v>
-      </c>
-      <c r="H131" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
+    </row>
+    <row r="170" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4160,10 +4545,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -4225,11 +4610,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4592,7 +4977,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B35" t="s">
         <v>48</v>
@@ -4603,7 +4988,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B36" t="s">
         <v>48</v>
@@ -4658,21 +5043,21 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>327</v>
       </c>
       <c r="B41" t="s">
-        <v>153</v>
+        <v>48</v>
       </c>
       <c r="C41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>250</v>
+        <v>154</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -4680,10 +5065,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B43" t="s">
-        <v>153</v>
+        <v>50</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -4691,10 +5076,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>251</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -4702,10 +5087,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -4713,7 +5098,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B46" t="s">
         <v>50</v>
@@ -4724,10 +5109,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -4735,32 +5120,29 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>283</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>281</v>
+      </c>
+      <c r="B49" t="s">
         <v>60</v>
       </c>
-      <c r="C48" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>169</v>
-      </c>
-      <c r="B50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" t="b">
-        <v>0</v>
-      </c>
-      <c r="D50" t="s">
-        <v>249</v>
+      <c r="C49" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
@@ -4768,10 +5150,13 @@
       <c r="C51" t="b">
         <v>0</v>
       </c>
+      <c r="D51" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B52" t="s">
         <v>50</v>
@@ -4782,12 +5167,23 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>233</v>
+        <v>173</v>
       </c>
       <c r="B53" t="s">
         <v>50</v>
       </c>
       <c r="C53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>233</v>
+      </c>
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates based on comments
</commit_message>
<xml_diff>
--- a/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
+++ b/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F704A4-4DCA-43A0-9F22-2951AC422C96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE8D319-516D-4E06-B9AE-A02F3A559BC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="353">
   <si>
     <t>setting_name</t>
   </si>
@@ -470,9 +470,6 @@
     <t>data("BCG") != null || data("VACINAS") !=1</t>
   </si>
   <si>
-    <t>(data("BCGDATA") != null &amp;&amp; adate.ageInYears(data("BCGDATA")) != -9999 &amp;&amp; adate.ageInYears(data("BCGDATA")) &lt; 2019) || data("BCG") != 1</t>
-  </si>
-  <si>
     <t>VACINASOU</t>
   </si>
   <si>
@@ -527,9 +524,6 @@
     <t>Correct</t>
   </si>
   <si>
-    <t>Corrigir</t>
-  </si>
-  <si>
     <t>Alterar</t>
   </si>
   <si>
@@ -587,9 +581,6 @@
     <t>data("NOMECRICON") == "2"</t>
   </si>
   <si>
-    <t>adate.display(data("DOB"))</t>
-  </si>
-  <si>
     <t>data("SEX") == "3" || data("SEX") == null</t>
   </si>
   <si>
@@ -608,9 +599,6 @@
     <t>data("POLIO") != null || data("VACINAS") !=1</t>
   </si>
   <si>
-    <t>(data("POLIODATA") != null &amp;&amp; adate.ageInYears(data("POLIODATA")) != -9999 &amp;&amp; adate.ageInYears(data("POLIODATA")) &lt; 2019) || data("POLIO") != 1</t>
-  </si>
-  <si>
     <t>data("VACINFO") != "3"</t>
   </si>
   <si>
@@ -626,24 +614,12 @@
     <t>OUTROVAC</t>
   </si>
   <si>
-    <t>What is the first vaccine the child received after polio or BCG?</t>
-  </si>
-  <si>
-    <t>Qual é a primeira vacina que a criança recebeu após a poliomielite ou BCG?</t>
-  </si>
-  <si>
     <t>data("OUTROVAC") != null || data("VACINASOU") !=1</t>
   </si>
   <si>
     <t>OUTRODATA</t>
   </si>
   <si>
-    <t>Date of first vaccine received after polio or BCG</t>
-  </si>
-  <si>
-    <t>Data da primeira vacina recebida após a poliomielite ou BCG</t>
-  </si>
-  <si>
     <t>Penta</t>
   </si>
   <si>
@@ -857,18 +833,6 @@
     <t>Existe algum adesivo ou número de identificação no cartão?</t>
   </si>
   <si>
-    <t>Measure of the mid-upper-arm circumference</t>
-  </si>
-  <si>
-    <t>Medida da circunferência do braço</t>
-  </si>
-  <si>
-    <t>If MUAC is less than 50mm write "11" &lt;/br&gt; If it is not possible to measure MUAC write "999"</t>
-  </si>
-  <si>
-    <t>Se o MUAC for menor que 50 mm, escreva "11" &lt;/br&gt; Se não for possível medir o MUAC, escreva "999"</t>
-  </si>
-  <si>
     <t>OBSCRI</t>
   </si>
   <si>
@@ -878,9 +842,6 @@
     <t>&lt;i&gt; Se você tiver algum comentário ou observação sobre a criança, escreva aqui &lt;/i&gt;</t>
   </si>
   <si>
-    <t>(data("OUTRODATA") != null &amp;&amp; adate.ageInYears(data("OUTRODATA")) != -9999 &amp;&amp; adate.ageInYears(data("OUTRODATA")) &lt; 2019) || data("VACINASOU") !=1</t>
-  </si>
-  <si>
     <t>data("SEX") != null || data("SEXCON") !=2</t>
   </si>
   <si>
@@ -890,18 +851,9 @@
     <t>displayREGDIA</t>
   </si>
   <si>
-    <t>adate.display(data("REGDIA"))</t>
-  </si>
-  <si>
     <t>(adate.diffInDays(data("DOB"),data("DATASEG")) &gt;= 0 &amp;&amp; adate.diffInDays(data("REGDIA"),data("DOB")) &gt;= 0 &amp;&amp; adate.ageInYears(data("DOB")) != -9999 &amp;&amp; adate.ageInYears(data("DOB")) &lt; 2019) || data("DOBCON") !=2</t>
   </si>
   <si>
-    <t>Date of birth is after today or before regdia:</t>
-  </si>
-  <si>
-    <t>A data de nascimento é depois de hoje ou antes do regdia:</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Follow-up on child {{data.NOMECRI}} regida: {{calculates.displayREGDIA}} &lt;/b&gt;</t>
   </si>
   <si>
@@ -930,9 +882,6 @@
   </si>
   <si>
     <t>poliocheck</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ((adate.diffInDays(data("DATASAICRI"),data("DATASEG")) &gt;= 0 || adate.dayUnknown(data("DATASAICRI"))) &amp;&amp; adate.ageInYears(data("DATASAICRI")) != -9999 &amp;&amp; adate.ageInYears(data("DATASAICRI")) &lt; 2019) || (data("ESTADOCRI") != 2 &amp;&amp; data("ESTADOCRI") != 3)</t>
   </si>
   <si>
     <t>((adate.diffInDays(data("DATASAIMUL"),data("DATASEG")) &gt;= 0 || adate.dayUnknown(data("DATASAIMUL"))) &amp;&amp; data("DATASAIMUL") != null &amp;&amp; adate.ageInYears(data("DATASAIMUL")) != -9999 &amp;&amp; adate.ageInYears(data("DATASAIMUL")) &lt; 2019) || (data("ESTADOMUL") != 2 &amp;&amp; data("ESTADOMUL") != 3)</t>
@@ -1096,6 +1045,54 @@
   </si>
   <si>
     <t>hideInContents</t>
+  </si>
+  <si>
+    <t>adate.display(data("BCGDATA"))</t>
+  </si>
+  <si>
+    <t>adate.display(data("POLIODATA"))</t>
+  </si>
+  <si>
+    <t>Date of birth is after today or before date of pregnancy registration:</t>
+  </si>
+  <si>
+    <t>A data de nascimento é depois de hoje ou antes do data de registro da gravidez:</t>
+  </si>
+  <si>
+    <t>Please use the measuring tape from BHP&lt;/br&gt; If MUAC is less than 50mm write "11" &lt;/br&gt; If it is not possible to measure MUAC write "999"</t>
+  </si>
+  <si>
+    <t>Certo</t>
+  </si>
+  <si>
+    <t>TELE</t>
+  </si>
+  <si>
+    <t>Por favor, use a fita métrica da PSB&lt;/br&gt; Se o MUAC for menor que 50 mm, escreva "11" &lt;/br&gt; Se não for possível medir o MUAC, escreva "999"</t>
+  </si>
+  <si>
+    <t>Measure of the mid-upper-arm circumference (left arm)</t>
+  </si>
+  <si>
+    <t>Medir de perímetro do esquerdo braço</t>
+  </si>
+  <si>
+    <t>What is the first other vaccines the child received?</t>
+  </si>
+  <si>
+    <t>Quais foram as primeiras outras vacinas que a criança recebeu?</t>
+  </si>
+  <si>
+    <t>data("OUTRODATA") != null || data("VACINASOU") !=1</t>
+  </si>
+  <si>
+    <t>((adate.diffInDays(data("DATASAICRI"),data("DATASEG")) &gt;= 0 || adate.dayUnknown(data("DATASAICRI"))) &amp;&amp; data("DATASAICRI") != null &amp;&amp; adate.ageInYears(data("DATASAICRI")) != -9999 &amp;&amp; adate.ageInYears(data("DATASAICRI")) &lt; 2019) || (data("ESTADOCRI") != 2 &amp;&amp; data("ESTADOCRI") != 3)</t>
+  </si>
+  <si>
+    <t>data("BCGDATA") != null || data("BCG") != 1</t>
+  </si>
+  <si>
+    <t>data("POLIODATA") != null  || data("POLIO") != 1</t>
   </si>
 </sst>
 </file>
@@ -1605,7 +1602,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B8" t="s">
         <v>74</v>
@@ -1624,9 +1621,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:S188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K180" sqref="K180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,7 +1705,7 @@
         <v>140</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1721,10 +1718,10 @@
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H3" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S3" t="b">
         <v>1</v>
@@ -1735,10 +1732,10 @@
         <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="H4" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="S4" t="b">
         <v>1</v>
@@ -1749,10 +1746,10 @@
         <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="H5" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="S5" t="b">
         <v>1</v>
@@ -1763,10 +1760,10 @@
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="H6" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="S6" t="b">
         <v>1</v>
@@ -1777,10 +1774,10 @@
         <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="H7" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
@@ -1794,10 +1791,10 @@
         <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="H8" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="S8" t="b">
         <v>1</v>
@@ -1808,10 +1805,10 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
       <c r="H9" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="S9" t="b">
         <v>1</v>
@@ -1832,10 +1829,10 @@
         <v>35</v>
       </c>
       <c r="G12" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H12" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S12" t="b">
         <v>1</v>
@@ -1879,10 +1876,10 @@
         <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H16" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S16" t="b">
         <v>1</v>
@@ -1896,13 +1893,13 @@
         <v>69</v>
       </c>
       <c r="F17" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="G17" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="H17" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="J17" t="b">
         <v>1</v>
@@ -1913,7 +1910,7 @@
         <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -1921,7 +1918,7 @@
         <v>28</v>
       </c>
       <c r="F19" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="G19" t="s">
         <v>142</v>
@@ -1930,13 +1927,13 @@
         <v>143</v>
       </c>
       <c r="K19" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="N19" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="O19" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="P19" t="b">
         <v>0</v>
@@ -1962,10 +1959,10 @@
         <v>35</v>
       </c>
       <c r="G23" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H23" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S23" t="b">
         <v>1</v>
@@ -1976,10 +1973,10 @@
         <v>35</v>
       </c>
       <c r="G24" t="s">
+        <v>159</v>
+      </c>
+      <c r="H24" t="s">
         <v>160</v>
-      </c>
-      <c r="H24" t="s">
-        <v>161</v>
       </c>
       <c r="S24" t="b">
         <v>1</v>
@@ -1990,25 +1987,25 @@
         <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F25" t="s">
+        <v>164</v>
+      </c>
+      <c r="G25" t="s">
+        <v>165</v>
+      </c>
+      <c r="H25" t="s">
         <v>166</v>
       </c>
-      <c r="G25" t="s">
-        <v>167</v>
-      </c>
-      <c r="H25" t="s">
-        <v>168</v>
-      </c>
       <c r="J25" t="b">
         <v>1</v>
       </c>
       <c r="L25" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="M25" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="S25" t="b">
         <v>1</v>
@@ -2019,7 +2016,7 @@
         <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
@@ -2036,7 +2033,7 @@
         <v>87</v>
       </c>
       <c r="K27" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
@@ -2059,10 +2056,10 @@
         <v>35</v>
       </c>
       <c r="G31" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H31" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S31" t="b">
         <v>1</v>
@@ -2073,10 +2070,10 @@
         <v>35</v>
       </c>
       <c r="G32" t="s">
+        <v>159</v>
+      </c>
+      <c r="H32" t="s">
         <v>160</v>
-      </c>
-      <c r="H32" t="s">
-        <v>161</v>
       </c>
       <c r="S32" t="b">
         <v>1</v>
@@ -2087,7 +2084,7 @@
         <v>67</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="2:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2095,10 +2092,10 @@
         <v>35</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I34"/>
       <c r="J34" t="b">
@@ -2118,7 +2115,7 @@
         <v>67</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="2:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2126,10 +2123,10 @@
         <v>35</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I37"/>
       <c r="J37" t="b">
@@ -2151,7 +2148,7 @@
         <v>67</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="40" spans="2:19" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2159,10 +2156,10 @@
         <v>35</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I40"/>
       <c r="J40" t="b">
@@ -2182,10 +2179,10 @@
         <v>50</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="S42" t="b">
         <v>1</v>
@@ -2196,7 +2193,7 @@
         <v>67</v>
       </c>
       <c r="C43" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.25">
@@ -2216,7 +2213,7 @@
         <v>90</v>
       </c>
       <c r="K44" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
@@ -2239,10 +2236,10 @@
         <v>35</v>
       </c>
       <c r="G48" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H48" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S48" t="b">
         <v>1</v>
@@ -2253,10 +2250,10 @@
         <v>35</v>
       </c>
       <c r="G49" t="s">
+        <v>159</v>
+      </c>
+      <c r="H49" t="s">
         <v>160</v>
-      </c>
-      <c r="H49" t="s">
-        <v>161</v>
       </c>
       <c r="S49" t="b">
         <v>1</v>
@@ -2267,16 +2264,16 @@
         <v>50</v>
       </c>
       <c r="E50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F50" t="s">
+        <v>168</v>
+      </c>
+      <c r="G50" t="s">
+        <v>169</v>
+      </c>
+      <c r="H50" t="s">
         <v>170</v>
-      </c>
-      <c r="G50" t="s">
-        <v>171</v>
-      </c>
-      <c r="H50" t="s">
-        <v>172</v>
       </c>
       <c r="J50" t="b">
         <v>1</v>
@@ -2290,7 +2287,7 @@
         <v>67</v>
       </c>
       <c r="C51" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.25">
@@ -2307,13 +2304,13 @@
         <v>92</v>
       </c>
       <c r="K52" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="N52" t="s">
-        <v>287</v>
+        <v>339</v>
       </c>
       <c r="O52" t="s">
-        <v>288</v>
+        <v>340</v>
       </c>
       <c r="P52" t="b">
         <v>0</v>
@@ -2340,10 +2337,10 @@
         <v>35</v>
       </c>
       <c r="G56" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H56" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S56" t="b">
         <v>1</v>
@@ -2382,7 +2379,7 @@
         <v>28</v>
       </c>
       <c r="F59" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G59" t="s">
         <v>142</v>
@@ -2391,13 +2388,13 @@
         <v>143</v>
       </c>
       <c r="K59" t="s">
-        <v>299</v>
+        <v>350</v>
       </c>
       <c r="N59" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="O59" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="P59" t="b">
         <v>0</v>
@@ -2423,10 +2420,10 @@
         <v>35</v>
       </c>
       <c r="G63" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H63" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S63" t="b">
         <v>1</v>
@@ -2477,7 +2474,7 @@
         <v>67</v>
       </c>
       <c r="C66" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
@@ -2485,16 +2482,16 @@
         <v>60</v>
       </c>
       <c r="F67" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="G67" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="H67" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="K67" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
@@ -2517,7 +2514,7 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="B71" t="s">
         <v>37</v>
@@ -2528,10 +2525,10 @@
         <v>35</v>
       </c>
       <c r="G72" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H72" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S72" t="b">
         <v>1</v>
@@ -2579,7 +2576,7 @@
         <v>129</v>
       </c>
       <c r="K75" t="s">
-        <v>145</v>
+        <v>351</v>
       </c>
       <c r="P75" t="b">
         <v>0</v>
@@ -2598,16 +2595,16 @@
         <v>52</v>
       </c>
       <c r="F77" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G77" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="H77" t="s">
         <v>130</v>
       </c>
       <c r="K77" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
@@ -2615,7 +2612,7 @@
         <v>67</v>
       </c>
       <c r="C78" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.25">
@@ -2623,7 +2620,7 @@
         <v>28</v>
       </c>
       <c r="F79" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G79" t="s">
         <v>128</v>
@@ -2632,7 +2629,7 @@
         <v>129</v>
       </c>
       <c r="K79" t="s">
-        <v>191</v>
+        <v>352</v>
       </c>
       <c r="P79" t="b">
         <v>0</v>
@@ -2648,15 +2645,15 @@
         <v>67</v>
       </c>
       <c r="C81" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="F82" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="I82">
         <v>2</v>
@@ -2675,15 +2672,15 @@
         <v>67</v>
       </c>
       <c r="C84" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="F85" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="I85">
         <v>2</v>
@@ -2707,12 +2704,12 @@
         <v>67</v>
       </c>
       <c r="C88" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="B89" t="s">
         <v>37</v>
@@ -2726,10 +2723,10 @@
         <v>35</v>
       </c>
       <c r="G90" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H90" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S90" t="b">
         <v>1</v>
@@ -2740,10 +2737,10 @@
         <v>35</v>
       </c>
       <c r="G91" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="H91" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="S91" t="b">
         <v>1</v>
@@ -2751,10 +2748,10 @@
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D92" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="F92" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="I92">
         <v>1</v>
@@ -2775,12 +2772,12 @@
         <v>67</v>
       </c>
       <c r="C95" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="B96" t="s">
         <v>37</v>
@@ -2791,10 +2788,10 @@
         <v>35</v>
       </c>
       <c r="G97" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H97" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S97" t="b">
         <v>1</v>
@@ -2805,10 +2802,10 @@
         <v>35</v>
       </c>
       <c r="G98" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="H98" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="S98" t="b">
         <v>1</v>
@@ -2816,10 +2813,10 @@
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="F99" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="I99">
         <v>1</v>
@@ -2843,12 +2840,12 @@
         <v>67</v>
       </c>
       <c r="C102" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
@@ -2866,10 +2863,10 @@
         <v>35</v>
       </c>
       <c r="G106" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H106" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S106" t="b">
         <v>1</v>
@@ -2883,16 +2880,16 @@
         <v>52</v>
       </c>
       <c r="F107" t="s">
+        <v>145</v>
+      </c>
+      <c r="G107" t="s">
         <v>146</v>
       </c>
-      <c r="G107" t="s">
+      <c r="H107" t="s">
         <v>147</v>
       </c>
-      <c r="H107" t="s">
+      <c r="K107" t="s">
         <v>148</v>
-      </c>
-      <c r="K107" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="108" spans="1:19" x14ac:dyDescent="0.25">
@@ -2905,12 +2902,12 @@
         <v>67</v>
       </c>
       <c r="C109" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="B110" t="s">
         <v>37</v>
@@ -2921,10 +2918,10 @@
         <v>35</v>
       </c>
       <c r="G111" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H111" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S111" t="b">
         <v>1</v>
@@ -2932,22 +2929,22 @@
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D112" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E112" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F112" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G112" t="s">
-        <v>197</v>
+        <v>347</v>
       </c>
       <c r="H112" t="s">
-        <v>198</v>
+        <v>348</v>
       </c>
       <c r="K112" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
@@ -2955,7 +2952,7 @@
         <v>67</v>
       </c>
       <c r="C113" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
@@ -2963,16 +2960,16 @@
         <v>60</v>
       </c>
       <c r="F114" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="G114" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="H114" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="K114" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
@@ -2985,16 +2982,16 @@
         <v>28</v>
       </c>
       <c r="F116" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="G116" t="s">
-        <v>201</v>
+        <v>128</v>
       </c>
       <c r="H116" t="s">
-        <v>202</v>
+        <v>129</v>
       </c>
       <c r="K116" t="s">
-        <v>281</v>
+        <v>349</v>
       </c>
       <c r="P116" t="b">
         <v>0</v>
@@ -3005,15 +3002,15 @@
         <v>67</v>
       </c>
       <c r="C117" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="F118" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="I118">
         <v>2</v>
@@ -3037,12 +3034,12 @@
         <v>67</v>
       </c>
       <c r="C121" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="B122" t="s">
         <v>37</v>
@@ -3053,10 +3050,10 @@
         <v>35</v>
       </c>
       <c r="G123" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="H123" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="S123" t="b">
         <v>1</v>
@@ -3067,10 +3064,10 @@
         <v>35</v>
       </c>
       <c r="G124" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="H124" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="S124" t="b">
         <v>1</v>
@@ -3078,10 +3075,10 @@
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
       <c r="F125" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="I125">
         <v>1</v>
@@ -3105,12 +3102,12 @@
         <v>67</v>
       </c>
       <c r="C128" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
     </row>
     <row r="129" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
     </row>
     <row r="130" spans="2:19" x14ac:dyDescent="0.25">
@@ -3133,7 +3130,7 @@
         <v>67</v>
       </c>
       <c r="C133" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="134" spans="2:19" x14ac:dyDescent="0.25">
@@ -3141,7 +3138,7 @@
         <v>67</v>
       </c>
       <c r="C134" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="135" spans="2:19" x14ac:dyDescent="0.25">
@@ -3154,10 +3151,10 @@
         <v>35</v>
       </c>
       <c r="G136" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H136" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S136" t="b">
         <v>1</v>
@@ -3165,25 +3162,25 @@
     </row>
     <row r="137" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D137" t="s">
+        <v>149</v>
+      </c>
+      <c r="F137" t="s">
         <v>150</v>
       </c>
-      <c r="F137" t="s">
+      <c r="G137" t="s">
         <v>151</v>
       </c>
-      <c r="G137" t="s">
+      <c r="H137" t="s">
         <v>152</v>
       </c>
-      <c r="H137" t="s">
+      <c r="L137" t="s">
         <v>153</v>
       </c>
-      <c r="L137" t="s">
+      <c r="M137" t="s">
         <v>154</v>
       </c>
-      <c r="M137" t="s">
+      <c r="R137" t="s">
         <v>155</v>
-      </c>
-      <c r="R137" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="138" spans="2:19" x14ac:dyDescent="0.25">
@@ -3206,10 +3203,10 @@
         <v>35</v>
       </c>
       <c r="G141" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H141" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S141" t="b">
         <v>1</v>
@@ -3223,19 +3220,19 @@
         <v>52</v>
       </c>
       <c r="F142" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="G142" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="H142" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="K142" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="R142" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="143" spans="2:19" x14ac:dyDescent="0.25">
@@ -3243,21 +3240,21 @@
         <v>67</v>
       </c>
       <c r="C143" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="144" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D144" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F144" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="G144" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="H144" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
     </row>
     <row r="145" spans="2:19" x14ac:dyDescent="0.25">
@@ -3280,7 +3277,7 @@
         <v>67</v>
       </c>
       <c r="C148" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
     </row>
     <row r="149" spans="2:19" x14ac:dyDescent="0.25">
@@ -3293,10 +3290,10 @@
         <v>35</v>
       </c>
       <c r="G150" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H150" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S150" t="b">
         <v>1</v>
@@ -3304,28 +3301,28 @@
     </row>
     <row r="151" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="F151" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="G151" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="H151" t="s">
-        <v>340</v>
+        <v>323</v>
       </c>
       <c r="K151" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="L151" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="M151" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
       <c r="R151" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
     </row>
     <row r="152" spans="2:19" x14ac:dyDescent="0.25">
@@ -3351,7 +3348,7 @@
         <v>67</v>
       </c>
       <c r="C155" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
     </row>
     <row r="156" spans="2:19" x14ac:dyDescent="0.25">
@@ -3364,10 +3361,10 @@
         <v>35</v>
       </c>
       <c r="G157" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="H157" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="S157" t="b">
         <v>1</v>
@@ -3381,16 +3378,16 @@
         <v>53</v>
       </c>
       <c r="F158" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="G158" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="H158" t="s">
-        <v>347</v>
+        <v>330</v>
       </c>
       <c r="K158" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
     </row>
     <row r="159" spans="2:19" x14ac:dyDescent="0.25">
@@ -3403,7 +3400,7 @@
         <v>67</v>
       </c>
       <c r="C160" t="s">
-        <v>348</v>
+        <v>331</v>
       </c>
     </row>
     <row r="161" spans="2:19" x14ac:dyDescent="0.25">
@@ -3416,10 +3413,10 @@
         <v>35</v>
       </c>
       <c r="G162" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="H162" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="S162" t="b">
         <v>1</v>
@@ -3427,28 +3424,28 @@
     </row>
     <row r="163" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="F163" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="G163" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="H163" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="K163" t="s">
-        <v>351</v>
+        <v>334</v>
       </c>
       <c r="L163" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="M163" t="s">
-        <v>339</v>
+        <v>322</v>
       </c>
       <c r="R163" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
     </row>
     <row r="164" spans="2:19" x14ac:dyDescent="0.25">
@@ -3476,10 +3473,10 @@
         <v>35</v>
       </c>
       <c r="G168" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H168" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S168" t="b">
         <v>1</v>
@@ -3493,28 +3490,28 @@
         <v>81</v>
       </c>
       <c r="G169" t="s">
-        <v>274</v>
+        <v>345</v>
       </c>
       <c r="H169" t="s">
-        <v>275</v>
+        <v>346</v>
       </c>
       <c r="K169" t="s">
+        <v>156</v>
+      </c>
+      <c r="L169" t="s">
+        <v>341</v>
+      </c>
+      <c r="M169" t="s">
+        <v>344</v>
+      </c>
+      <c r="N169" t="s">
         <v>157</v>
       </c>
-      <c r="L169" t="s">
-        <v>276</v>
-      </c>
-      <c r="M169" t="s">
-        <v>277</v>
-      </c>
-      <c r="N169" t="s">
+      <c r="O169" t="s">
         <v>158</v>
       </c>
-      <c r="O169" t="s">
-        <v>159</v>
-      </c>
       <c r="R169" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
     </row>
     <row r="170" spans="2:19" x14ac:dyDescent="0.25">
@@ -3532,10 +3529,10 @@
         <v>35</v>
       </c>
       <c r="G172" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H172" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S172" t="b">
         <v>1</v>
@@ -3558,16 +3555,16 @@
         <v>124</v>
       </c>
       <c r="K173" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="L173" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="M173" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="R173" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
     </row>
     <row r="174" spans="2:19" x14ac:dyDescent="0.25">
@@ -3590,10 +3587,10 @@
         <v>35</v>
       </c>
       <c r="G177" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H177" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S177" t="b">
         <v>1</v>
@@ -3610,19 +3607,19 @@
         <v>83</v>
       </c>
       <c r="G178" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="H178" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="J178" t="b">
         <v>1</v>
       </c>
       <c r="L178" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="M178" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
     </row>
     <row r="179" spans="2:19" x14ac:dyDescent="0.25">
@@ -3647,13 +3644,13 @@
         <v>133</v>
       </c>
       <c r="K180" s="20" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="N180" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="O180" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="P180" t="b">
         <v>0</v>
@@ -3679,10 +3676,10 @@
         <v>35</v>
       </c>
       <c r="G184" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="H184" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="S184" t="b">
         <v>1</v>
@@ -3693,10 +3690,10 @@
         <v>35</v>
       </c>
       <c r="G185" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="H185" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="S185" t="b">
         <v>1</v>
@@ -3707,10 +3704,10 @@
         <v>35</v>
       </c>
       <c r="G186" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="H186" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="S186" t="b">
         <v>1</v>
@@ -3721,13 +3718,13 @@
         <v>60</v>
       </c>
       <c r="F187" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="G187" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="H187" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
     </row>
     <row r="188" spans="2:19" x14ac:dyDescent="0.25">
@@ -3746,8 +3743,8 @@
   <dimension ref="A1:F146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37:D37"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3774,32 +3771,32 @@
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" s="11" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>164</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="11" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4147,10 +4144,10 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D30" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4161,86 +4158,86 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" t="s">
         <v>195</v>
       </c>
-      <c r="B32" t="s">
-        <v>203</v>
-      </c>
       <c r="C32" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D32" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B33" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C33" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D33" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B34" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C34" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D34" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B35" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C35" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="D35" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B36" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C36" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D36" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B37" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="C37" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D37" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4891,7 +4888,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:B3"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4910,18 +4907,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>184</v>
+        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>285</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -4983,11 +4980,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46:C46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5023,7 +5020,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5094,7 +5091,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
@@ -5105,7 +5102,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
         <v>60</v>
@@ -5114,23 +5111,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>242</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>343</v>
+      </c>
+      <c r="B11" t="s">
         <v>60</v>
       </c>
-      <c r="C12" t="b">
+      <c r="C11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>234</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -5138,10 +5135,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>243</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -5152,7 +5149,7 @@
         <v>235</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -5160,68 +5157,68 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>244</v>
-      </c>
-      <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" t="b">
+      <c r="C17" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>246</v>
+      </c>
+      <c r="B20" t="s">
         <v>50</v>
       </c>
-      <c r="C19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>255</v>
-      </c>
-      <c r="B21" t="s">
-        <v>256</v>
-      </c>
-      <c r="C21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>245</v>
+      <c r="C20" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>247</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>248</v>
       </c>
       <c r="C22" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -5229,10 +5226,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -5240,10 +5237,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -5251,10 +5248,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -5262,10 +5259,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>232</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -5273,10 +5270,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>224</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -5284,7 +5281,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="B29" t="s">
         <v>50</v>
@@ -5295,10 +5292,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>259</v>
+        <v>79</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -5306,10 +5303,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>251</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -5317,10 +5314,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -5328,10 +5325,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -5339,10 +5336,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -5350,18 +5347,18 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>297</v>
+        <v>186</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="B36" t="s">
         <v>48</v>
@@ -5372,21 +5369,21 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>146</v>
+        <v>282</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>196</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
-        <v>194</v>
+        <v>50</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -5394,10 +5391,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>265</v>
+        <v>192</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>190</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -5405,10 +5402,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>200</v>
+        <v>257</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -5416,32 +5413,32 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>321</v>
+        <v>194</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>304</v>
       </c>
       <c r="B42" t="s">
-        <v>150</v>
+        <v>48</v>
       </c>
       <c r="C42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>247</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>149</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -5449,10 +5446,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B44" t="s">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -5460,10 +5457,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>331</v>
+        <v>240</v>
       </c>
       <c r="B45" t="s">
-        <v>330</v>
+        <v>149</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -5471,10 +5468,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>344</v>
+        <v>314</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>313</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -5482,10 +5479,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>327</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -5493,10 +5490,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
@@ -5504,7 +5501,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B49" t="s">
         <v>50</v>
@@ -5515,10 +5512,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="C50" t="b">
         <v>0</v>
@@ -5526,32 +5523,29 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>278</v>
+        <v>84</v>
       </c>
       <c r="B51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>266</v>
+      </c>
+      <c r="B52" t="s">
         <v>60</v>
       </c>
-      <c r="C51" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>166</v>
-      </c>
-      <c r="B53" t="s">
-        <v>50</v>
-      </c>
-      <c r="C53" t="b">
-        <v>0</v>
-      </c>
-      <c r="D53" t="s">
-        <v>246</v>
+      <c r="C52" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B54" t="s">
         <v>50</v>
@@ -5559,10 +5553,13 @@
       <c r="C54" t="b">
         <v>0</v>
       </c>
+      <c r="D54" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B55" t="s">
         <v>50</v>
@@ -5573,17 +5570,29 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>230</v>
+        <v>168</v>
       </c>
       <c r="B56" t="s">
         <v>50</v>
       </c>
       <c r="C56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>222</v>
+      </c>
+      <c r="B57" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added reason for hosp
</commit_message>
<xml_diff>
--- a/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
+++ b/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F920D14C-6B92-4849-9DC5-4A448836BFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C7E800-E52B-49B8-8F59-6AE99A0216A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="357">
   <si>
     <t>setting_name</t>
   </si>
@@ -1093,6 +1093,18 @@
   </si>
   <si>
     <t>Estado da criança</t>
+  </si>
+  <si>
+    <t>HOSPREASON</t>
+  </si>
+  <si>
+    <t>What happened? / Why did the child get hospitalised?</t>
+  </si>
+  <si>
+    <t>O que aconteceu? / Por que a criança foi hospitalizada?</t>
+  </si>
+  <si>
+    <t>data("HOSPREASON") != null || data("HOSP") != 1</t>
   </si>
 </sst>
 </file>
@@ -1619,11 +1631,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:S188"/>
+  <dimension ref="A1:S189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K181" sqref="K181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3657,32 +3669,35 @@
       </c>
     </row>
     <row r="181" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B181" t="s">
-        <v>68</v>
+      <c r="D181" t="s">
+        <v>60</v>
+      </c>
+      <c r="F181" t="s">
+        <v>353</v>
+      </c>
+      <c r="G181" t="s">
+        <v>354</v>
+      </c>
+      <c r="H181" t="s">
+        <v>355</v>
+      </c>
+      <c r="K181" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="182" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="183" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="184" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="184" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="D184" t="s">
-        <v>35</v>
-      </c>
-      <c r="G184" t="s">
-        <v>272</v>
-      </c>
-      <c r="H184" t="s">
-        <v>273</v>
-      </c>
-      <c r="S184" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="185" spans="2:19" x14ac:dyDescent="0.25">
@@ -3690,10 +3705,10 @@
         <v>35</v>
       </c>
       <c r="G185" t="s">
-        <v>208</v>
+        <v>272</v>
       </c>
       <c r="H185" t="s">
-        <v>209</v>
+        <v>273</v>
       </c>
       <c r="S185" t="b">
         <v>1</v>
@@ -3704,10 +3719,10 @@
         <v>35</v>
       </c>
       <c r="G186" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H186" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="S186" t="b">
         <v>1</v>
@@ -3715,20 +3730,34 @@
     </row>
     <row r="187" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
+        <v>35</v>
+      </c>
+      <c r="G187" t="s">
+        <v>210</v>
+      </c>
+      <c r="H187" t="s">
+        <v>211</v>
+      </c>
+      <c r="S187" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="D188" t="s">
         <v>60</v>
       </c>
-      <c r="F187" t="s">
+      <c r="F188" t="s">
         <v>265</v>
       </c>
-      <c r="G187" t="s">
+      <c r="G188" t="s">
         <v>266</v>
       </c>
-      <c r="H187" t="s">
+      <c r="H188" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="188" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B188" t="s">
+    <row r="189" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4980,11 +5009,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D1048576"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5534,7 +5563,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>265</v>
+        <v>353</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>
@@ -5543,23 +5572,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>163</v>
-      </c>
-      <c r="B54" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" t="b">
-        <v>0</v>
-      </c>
-      <c r="D54" t="s">
-        <v>237</v>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>265</v>
+      </c>
+      <c r="B53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B55" t="s">
         <v>50</v>
@@ -5567,10 +5593,13 @@
       <c r="C55" t="b">
         <v>0</v>
       </c>
+      <c r="D55" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B56" t="s">
         <v>50</v>
@@ -5581,12 +5610,23 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>221</v>
+        <v>167</v>
       </c>
       <c r="B57" t="s">
         <v>50</v>
       </c>
       <c r="C57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>221</v>
+      </c>
+      <c r="B58" t="s">
+        <v>50</v>
+      </c>
+      <c r="C58" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes to "Already have card"
</commit_message>
<xml_diff>
--- a/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
+++ b/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFD84D2-C21C-4CB6-BBE7-F4B8B454C980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A637BD85-3AE6-4EEB-A741-A37EA1E9A588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -1008,12 +1008,6 @@
     <t>data("VACINFO") != "1"</t>
   </si>
   <si>
-    <t>Has the child received a vaccination card?</t>
-  </si>
-  <si>
-    <t>A criança recebeu cartão de vacinação?</t>
-  </si>
-  <si>
     <t>data("HAVECARD") == "2"</t>
   </si>
   <si>
@@ -1102,6 +1096,12 @@
   </si>
   <si>
     <t>data("HOSPREASON") != null || data("HOSP") != 1</t>
+  </si>
+  <si>
+    <t>Has the child received a vaccination card from the health centre?</t>
+  </si>
+  <si>
+    <t>A criança recebeu cartão de vacinação do centro de saúde?</t>
   </si>
 </sst>
 </file>
@@ -1630,9 +1630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:S189"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F172" sqref="F172"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G158" sqref="G158:H158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,7 +1714,7 @@
         <v>139</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -2316,10 +2316,10 @@
         <v>270</v>
       </c>
       <c r="N52" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="O52" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="P52" t="b">
         <v>0</v>
@@ -2369,7 +2369,7 @@
         <v>88</v>
       </c>
       <c r="H57" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J57" t="b">
         <v>1</v>
@@ -2397,7 +2397,7 @@
         <v>142</v>
       </c>
       <c r="K59" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="N59" t="s">
         <v>273</v>
@@ -2585,7 +2585,7 @@
         <v>128</v>
       </c>
       <c r="K75" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="P75" t="b">
         <v>0</v>
@@ -2638,7 +2638,7 @@
         <v>128</v>
       </c>
       <c r="K79" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="P79" t="b">
         <v>0</v>
@@ -2713,7 +2713,7 @@
         <v>67</v>
       </c>
       <c r="C88" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
@@ -2781,7 +2781,7 @@
         <v>67</v>
       </c>
       <c r="C95" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
@@ -2947,10 +2947,10 @@
         <v>191</v>
       </c>
       <c r="G112" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="H112" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="K112" t="s">
         <v>192</v>
@@ -3000,7 +3000,7 @@
         <v>128</v>
       </c>
       <c r="K116" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="P116" t="b">
         <v>0</v>
@@ -3043,7 +3043,7 @@
         <v>67</v>
       </c>
       <c r="C121" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
@@ -3390,13 +3390,13 @@
         <v>322</v>
       </c>
       <c r="G158" t="s">
-        <v>324</v>
+        <v>354</v>
       </c>
       <c r="H158" t="s">
-        <v>325</v>
+        <v>355</v>
       </c>
       <c r="K158" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="159" spans="2:19" x14ac:dyDescent="0.25">
@@ -3409,7 +3409,7 @@
         <v>67</v>
       </c>
       <c r="C160" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="161" spans="2:19" x14ac:dyDescent="0.25">
@@ -3439,13 +3439,13 @@
         <v>309</v>
       </c>
       <c r="G163" t="s">
+        <v>325</v>
+      </c>
+      <c r="H163" t="s">
+        <v>326</v>
+      </c>
+      <c r="K163" t="s">
         <v>327</v>
-      </c>
-      <c r="H163" t="s">
-        <v>328</v>
-      </c>
-      <c r="K163" t="s">
-        <v>329</v>
       </c>
       <c r="L163" t="s">
         <v>316</v>
@@ -3499,19 +3499,19 @@
         <v>81</v>
       </c>
       <c r="G169" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="H169" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K169" t="s">
         <v>155</v>
       </c>
       <c r="L169" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="M169" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="N169" t="s">
         <v>156</v>
@@ -3670,16 +3670,16 @@
         <v>60</v>
       </c>
       <c r="F181" t="s">
+        <v>350</v>
+      </c>
+      <c r="G181" t="s">
+        <v>351</v>
+      </c>
+      <c r="H181" t="s">
         <v>352</v>
       </c>
-      <c r="G181" t="s">
+      <c r="K181" t="s">
         <v>353</v>
-      </c>
-      <c r="H181" t="s">
-        <v>354</v>
-      </c>
-      <c r="K181" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="182" spans="2:19" x14ac:dyDescent="0.25">
@@ -3807,7 +3807,7 @@
         <v>161</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4936,7 +4936,7 @@
         <v>182</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4944,7 +4944,7 @@
         <v>269</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -5008,7 +5008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
     </sheetView>
@@ -5139,7 +5139,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B11" t="s">
         <v>60</v>
@@ -5560,7 +5560,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
removed reg < dob constraint on DOB
</commit_message>
<xml_diff>
--- a/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
+++ b/app/config/tables/CHILDREN/Forms/CHILDFU/CHILDFU.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A637BD85-3AE6-4EEB-A741-A37EA1E9A588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD40F3F6-7D93-4235-BFA3-3E6562F37297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -845,9 +845,6 @@
     <t>displayREGDIA</t>
   </si>
   <si>
-    <t>(adate.diffInDays(data("DOB"),data("DATASEG")) &gt;= 0 &amp;&amp; adate.diffInDays(data("REGDIA"),data("DOB")) &gt;= 0 &amp;&amp; adate.ageInYears(data("DOB")) != -9999 &amp;&amp; adate.ageInYears(data("DOB")) &lt; 2019) || data("DOBCON") !=2</t>
-  </si>
-  <si>
     <t>&lt;b&gt;Follow-up on child {{data.NOMECRI}} regida: {{calculates.displayREGDIA}} &lt;/b&gt;</t>
   </si>
   <si>
@@ -1102,6 +1099,9 @@
   </si>
   <si>
     <t>A criança recebeu cartão de vacinação do centro de saúde?</t>
+  </si>
+  <si>
+    <t>(adate.diffInDays(data("DOB"),data("DATASEG")) &gt;= 0 &amp;&amp; adate.ageInYears(data("DOB")) != -9999 &amp;&amp; adate.ageInYears(data("DOB")) &lt; 2019) || data("DOBCON") !=2</t>
   </si>
 </sst>
 </file>
@@ -1630,9 +1630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:S189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G158" sqref="G158:H158"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,7 +1714,7 @@
         <v>139</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1727,10 +1727,10 @@
         <v>35</v>
       </c>
       <c r="G3" t="s">
+        <v>270</v>
+      </c>
+      <c r="H3" t="s">
         <v>271</v>
-      </c>
-      <c r="H3" t="s">
-        <v>272</v>
       </c>
       <c r="S3" t="b">
         <v>1</v>
@@ -1814,10 +1814,10 @@
         <v>35</v>
       </c>
       <c r="G9" t="s">
+        <v>319</v>
+      </c>
+      <c r="H9" t="s">
         <v>320</v>
-      </c>
-      <c r="H9" t="s">
-        <v>321</v>
       </c>
       <c r="S9" t="b">
         <v>1</v>
@@ -1838,10 +1838,10 @@
         <v>35</v>
       </c>
       <c r="G12" t="s">
+        <v>270</v>
+      </c>
+      <c r="H12" t="s">
         <v>271</v>
-      </c>
-      <c r="H12" t="s">
-        <v>272</v>
       </c>
       <c r="S12" t="b">
         <v>1</v>
@@ -1885,10 +1885,10 @@
         <v>35</v>
       </c>
       <c r="G16" t="s">
+        <v>270</v>
+      </c>
+      <c r="H16" t="s">
         <v>271</v>
-      </c>
-      <c r="H16" t="s">
-        <v>272</v>
       </c>
       <c r="S16" t="b">
         <v>1</v>
@@ -1936,13 +1936,13 @@
         <v>142</v>
       </c>
       <c r="K19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N19" t="s">
+        <v>272</v>
+      </c>
+      <c r="O19" t="s">
         <v>273</v>
-      </c>
-      <c r="O19" t="s">
-        <v>274</v>
       </c>
       <c r="P19" t="b">
         <v>0</v>
@@ -1968,10 +1968,10 @@
         <v>35</v>
       </c>
       <c r="G23" t="s">
+        <v>270</v>
+      </c>
+      <c r="H23" t="s">
         <v>271</v>
-      </c>
-      <c r="H23" t="s">
-        <v>272</v>
       </c>
       <c r="S23" t="b">
         <v>1</v>
@@ -2065,10 +2065,10 @@
         <v>35</v>
       </c>
       <c r="G31" t="s">
+        <v>270</v>
+      </c>
+      <c r="H31" t="s">
         <v>271</v>
-      </c>
-      <c r="H31" t="s">
-        <v>272</v>
       </c>
       <c r="S31" t="b">
         <v>1</v>
@@ -2245,10 +2245,10 @@
         <v>35</v>
       </c>
       <c r="G48" t="s">
+        <v>270</v>
+      </c>
+      <c r="H48" t="s">
         <v>271</v>
-      </c>
-      <c r="H48" t="s">
-        <v>272</v>
       </c>
       <c r="S48" t="b">
         <v>1</v>
@@ -2313,13 +2313,13 @@
         <v>92</v>
       </c>
       <c r="K52" t="s">
-        <v>270</v>
+        <v>355</v>
       </c>
       <c r="N52" t="s">
+        <v>329</v>
+      </c>
+      <c r="O52" t="s">
         <v>330</v>
-      </c>
-      <c r="O52" t="s">
-        <v>331</v>
       </c>
       <c r="P52" t="b">
         <v>0</v>
@@ -2346,10 +2346,10 @@
         <v>35</v>
       </c>
       <c r="G56" t="s">
+        <v>270</v>
+      </c>
+      <c r="H56" t="s">
         <v>271</v>
-      </c>
-      <c r="H56" t="s">
-        <v>272</v>
       </c>
       <c r="S56" t="b">
         <v>1</v>
@@ -2369,7 +2369,7 @@
         <v>88</v>
       </c>
       <c r="H57" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J57" t="b">
         <v>1</v>
@@ -2397,13 +2397,13 @@
         <v>142</v>
       </c>
       <c r="K59" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N59" t="s">
+        <v>272</v>
+      </c>
+      <c r="O59" t="s">
         <v>273</v>
-      </c>
-      <c r="O59" t="s">
-        <v>274</v>
       </c>
       <c r="P59" t="b">
         <v>0</v>
@@ -2429,10 +2429,10 @@
         <v>35</v>
       </c>
       <c r="G63" t="s">
+        <v>270</v>
+      </c>
+      <c r="H63" t="s">
         <v>271</v>
-      </c>
-      <c r="H63" t="s">
-        <v>272</v>
       </c>
       <c r="S63" t="b">
         <v>1</v>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B71" t="s">
         <v>37</v>
@@ -2534,10 +2534,10 @@
         <v>35</v>
       </c>
       <c r="G72" t="s">
+        <v>270</v>
+      </c>
+      <c r="H72" t="s">
         <v>271</v>
-      </c>
-      <c r="H72" t="s">
-        <v>272</v>
       </c>
       <c r="S72" t="b">
         <v>1</v>
@@ -2585,7 +2585,7 @@
         <v>128</v>
       </c>
       <c r="K75" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="P75" t="b">
         <v>0</v>
@@ -2607,7 +2607,7 @@
         <v>184</v>
       </c>
       <c r="G77" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H77" t="s">
         <v>129</v>
@@ -2638,7 +2638,7 @@
         <v>128</v>
       </c>
       <c r="K79" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="P79" t="b">
         <v>0</v>
@@ -2654,15 +2654,15 @@
         <v>67</v>
       </c>
       <c r="C81" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F82" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I82">
         <v>2</v>
@@ -2681,15 +2681,15 @@
         <v>67</v>
       </c>
       <c r="C84" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F85" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I85">
         <v>2</v>
@@ -2713,12 +2713,12 @@
         <v>67</v>
       </c>
       <c r="C88" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B89" t="s">
         <v>37</v>
@@ -2732,10 +2732,10 @@
         <v>35</v>
       </c>
       <c r="G90" t="s">
+        <v>270</v>
+      </c>
+      <c r="H90" t="s">
         <v>271</v>
-      </c>
-      <c r="H90" t="s">
-        <v>272</v>
       </c>
       <c r="S90" t="b">
         <v>1</v>
@@ -2746,10 +2746,10 @@
         <v>35</v>
       </c>
       <c r="G91" t="s">
+        <v>291</v>
+      </c>
+      <c r="H91" t="s">
         <v>292</v>
-      </c>
-      <c r="H91" t="s">
-        <v>293</v>
       </c>
       <c r="S91" t="b">
         <v>1</v>
@@ -2757,10 +2757,10 @@
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D92" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F92" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I92">
         <v>1</v>
@@ -2781,12 +2781,12 @@
         <v>67</v>
       </c>
       <c r="C95" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B96" t="s">
         <v>37</v>
@@ -2797,10 +2797,10 @@
         <v>35</v>
       </c>
       <c r="G97" t="s">
+        <v>270</v>
+      </c>
+      <c r="H97" t="s">
         <v>271</v>
-      </c>
-      <c r="H97" t="s">
-        <v>272</v>
       </c>
       <c r="S97" t="b">
         <v>1</v>
@@ -2811,10 +2811,10 @@
         <v>35</v>
       </c>
       <c r="G98" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H98" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="S98" t="b">
         <v>1</v>
@@ -2822,10 +2822,10 @@
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F99" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I99">
         <v>1</v>
@@ -2849,12 +2849,12 @@
         <v>67</v>
       </c>
       <c r="C102" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
@@ -2872,10 +2872,10 @@
         <v>35</v>
       </c>
       <c r="G106" t="s">
+        <v>270</v>
+      </c>
+      <c r="H106" t="s">
         <v>271</v>
-      </c>
-      <c r="H106" t="s">
-        <v>272</v>
       </c>
       <c r="S106" t="b">
         <v>1</v>
@@ -2916,7 +2916,7 @@
     </row>
     <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B110" t="s">
         <v>37</v>
@@ -2927,10 +2927,10 @@
         <v>35</v>
       </c>
       <c r="G111" t="s">
+        <v>270</v>
+      </c>
+      <c r="H111" t="s">
         <v>271</v>
-      </c>
-      <c r="H111" t="s">
-        <v>272</v>
       </c>
       <c r="S111" t="b">
         <v>1</v>
@@ -2947,10 +2947,10 @@
         <v>191</v>
       </c>
       <c r="G112" t="s">
+        <v>337</v>
+      </c>
+      <c r="H112" t="s">
         <v>338</v>
-      </c>
-      <c r="H112" t="s">
-        <v>339</v>
       </c>
       <c r="K112" t="s">
         <v>192</v>
@@ -3000,7 +3000,7 @@
         <v>128</v>
       </c>
       <c r="K116" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P116" t="b">
         <v>0</v>
@@ -3011,15 +3011,15 @@
         <v>67</v>
       </c>
       <c r="C117" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F118" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I118">
         <v>2</v>
@@ -3043,12 +3043,12 @@
         <v>67</v>
       </c>
       <c r="C121" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B122" t="s">
         <v>37</v>
@@ -3059,10 +3059,10 @@
         <v>35</v>
       </c>
       <c r="G123" t="s">
+        <v>289</v>
+      </c>
+      <c r="H123" t="s">
         <v>290</v>
-      </c>
-      <c r="H123" t="s">
-        <v>291</v>
       </c>
       <c r="S123" t="b">
         <v>1</v>
@@ -3073,10 +3073,10 @@
         <v>35</v>
       </c>
       <c r="G124" t="s">
+        <v>301</v>
+      </c>
+      <c r="H124" t="s">
         <v>302</v>
-      </c>
-      <c r="H124" t="s">
-        <v>303</v>
       </c>
       <c r="S124" t="b">
         <v>1</v>
@@ -3084,10 +3084,10 @@
     </row>
     <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F125" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I125">
         <v>1</v>
@@ -3111,12 +3111,12 @@
         <v>67</v>
       </c>
       <c r="C128" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="129" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="130" spans="2:19" x14ac:dyDescent="0.25">
@@ -3160,10 +3160,10 @@
         <v>35</v>
       </c>
       <c r="G136" t="s">
+        <v>270</v>
+      </c>
+      <c r="H136" t="s">
         <v>271</v>
-      </c>
-      <c r="H136" t="s">
-        <v>272</v>
       </c>
       <c r="S136" t="b">
         <v>1</v>
@@ -3212,10 +3212,10 @@
         <v>35</v>
       </c>
       <c r="G141" t="s">
+        <v>270</v>
+      </c>
+      <c r="H141" t="s">
         <v>271</v>
-      </c>
-      <c r="H141" t="s">
-        <v>272</v>
       </c>
       <c r="S141" t="b">
         <v>1</v>
@@ -3286,7 +3286,7 @@
         <v>67</v>
       </c>
       <c r="C148" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="149" spans="2:19" x14ac:dyDescent="0.25">
@@ -3299,10 +3299,10 @@
         <v>35</v>
       </c>
       <c r="G150" t="s">
+        <v>270</v>
+      </c>
+      <c r="H150" t="s">
         <v>271</v>
-      </c>
-      <c r="H150" t="s">
-        <v>272</v>
       </c>
       <c r="S150" t="b">
         <v>1</v>
@@ -3310,28 +3310,28 @@
     </row>
     <row r="151" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
+        <v>307</v>
+      </c>
+      <c r="F151" t="s">
         <v>308</v>
       </c>
-      <c r="F151" t="s">
+      <c r="G151" t="s">
+        <v>318</v>
+      </c>
+      <c r="H151" t="s">
+        <v>317</v>
+      </c>
+      <c r="K151" t="s">
         <v>309</v>
       </c>
-      <c r="G151" t="s">
-        <v>319</v>
-      </c>
-      <c r="H151" t="s">
-        <v>318</v>
-      </c>
-      <c r="K151" t="s">
-        <v>310</v>
-      </c>
       <c r="L151" t="s">
+        <v>315</v>
+      </c>
+      <c r="M151" t="s">
         <v>316</v>
       </c>
-      <c r="M151" t="s">
-        <v>317</v>
-      </c>
       <c r="R151" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="152" spans="2:19" x14ac:dyDescent="0.25">
@@ -3357,7 +3357,7 @@
         <v>67</v>
       </c>
       <c r="C155" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="156" spans="2:19" x14ac:dyDescent="0.25">
@@ -3370,10 +3370,10 @@
         <v>35</v>
       </c>
       <c r="G157" t="s">
+        <v>289</v>
+      </c>
+      <c r="H157" t="s">
         <v>290</v>
-      </c>
-      <c r="H157" t="s">
-        <v>291</v>
       </c>
       <c r="S157" t="b">
         <v>1</v>
@@ -3387,16 +3387,16 @@
         <v>53</v>
       </c>
       <c r="F158" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G158" t="s">
+        <v>353</v>
+      </c>
+      <c r="H158" t="s">
         <v>354</v>
       </c>
-      <c r="H158" t="s">
-        <v>355</v>
-      </c>
       <c r="K158" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="159" spans="2:19" x14ac:dyDescent="0.25">
@@ -3409,7 +3409,7 @@
         <v>67</v>
       </c>
       <c r="C160" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="161" spans="2:19" x14ac:dyDescent="0.25">
@@ -3422,10 +3422,10 @@
         <v>35</v>
       </c>
       <c r="G162" t="s">
+        <v>289</v>
+      </c>
+      <c r="H162" t="s">
         <v>290</v>
-      </c>
-      <c r="H162" t="s">
-        <v>291</v>
       </c>
       <c r="S162" t="b">
         <v>1</v>
@@ -3433,28 +3433,28 @@
     </row>
     <row r="163" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
+        <v>307</v>
+      </c>
+      <c r="F163" t="s">
         <v>308</v>
       </c>
-      <c r="F163" t="s">
-        <v>309</v>
-      </c>
       <c r="G163" t="s">
+        <v>324</v>
+      </c>
+      <c r="H163" t="s">
         <v>325</v>
       </c>
-      <c r="H163" t="s">
+      <c r="K163" t="s">
         <v>326</v>
       </c>
-      <c r="K163" t="s">
-        <v>327</v>
-      </c>
       <c r="L163" t="s">
+        <v>315</v>
+      </c>
+      <c r="M163" t="s">
         <v>316</v>
       </c>
-      <c r="M163" t="s">
-        <v>317</v>
-      </c>
       <c r="R163" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="164" spans="2:19" x14ac:dyDescent="0.25">
@@ -3482,10 +3482,10 @@
         <v>35</v>
       </c>
       <c r="G168" t="s">
+        <v>270</v>
+      </c>
+      <c r="H168" t="s">
         <v>271</v>
-      </c>
-      <c r="H168" t="s">
-        <v>272</v>
       </c>
       <c r="S168" t="b">
         <v>1</v>
@@ -3499,19 +3499,19 @@
         <v>81</v>
       </c>
       <c r="G169" t="s">
+        <v>335</v>
+      </c>
+      <c r="H169" t="s">
         <v>336</v>
-      </c>
-      <c r="H169" t="s">
-        <v>337</v>
       </c>
       <c r="K169" t="s">
         <v>155</v>
       </c>
       <c r="L169" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M169" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N169" t="s">
         <v>156</v>
@@ -3520,7 +3520,7 @@
         <v>157</v>
       </c>
       <c r="R169" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="170" spans="2:19" x14ac:dyDescent="0.25">
@@ -3538,10 +3538,10 @@
         <v>35</v>
       </c>
       <c r="G172" t="s">
+        <v>270</v>
+      </c>
+      <c r="H172" t="s">
         <v>271</v>
-      </c>
-      <c r="H172" t="s">
-        <v>272</v>
       </c>
       <c r="S172" t="b">
         <v>1</v>
@@ -3567,13 +3567,13 @@
         <v>247</v>
       </c>
       <c r="L173" t="s">
+        <v>304</v>
+      </c>
+      <c r="M173" t="s">
         <v>305</v>
       </c>
-      <c r="M173" t="s">
-        <v>306</v>
-      </c>
       <c r="R173" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="174" spans="2:19" x14ac:dyDescent="0.25">
@@ -3596,10 +3596,10 @@
         <v>35</v>
       </c>
       <c r="G177" t="s">
+        <v>270</v>
+      </c>
+      <c r="H177" t="s">
         <v>271</v>
-      </c>
-      <c r="H177" t="s">
-        <v>272</v>
       </c>
       <c r="S177" t="b">
         <v>1</v>
@@ -3616,19 +3616,19 @@
         <v>83</v>
       </c>
       <c r="G178" t="s">
+        <v>276</v>
+      </c>
+      <c r="H178" t="s">
         <v>277</v>
       </c>
-      <c r="H178" t="s">
-        <v>278</v>
-      </c>
       <c r="J178" t="b">
         <v>1</v>
       </c>
       <c r="L178" t="s">
+        <v>312</v>
+      </c>
+      <c r="M178" t="s">
         <v>313</v>
-      </c>
-      <c r="M178" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="179" spans="2:19" x14ac:dyDescent="0.25">
@@ -3653,13 +3653,13 @@
         <v>132</v>
       </c>
       <c r="K180" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N180" t="s">
+        <v>274</v>
+      </c>
+      <c r="O180" t="s">
         <v>275</v>
-      </c>
-      <c r="O180" t="s">
-        <v>276</v>
       </c>
       <c r="P180" t="b">
         <v>0</v>
@@ -3670,16 +3670,16 @@
         <v>60</v>
       </c>
       <c r="F181" t="s">
+        <v>349</v>
+      </c>
+      <c r="G181" t="s">
         <v>350</v>
       </c>
-      <c r="G181" t="s">
+      <c r="H181" t="s">
         <v>351</v>
       </c>
-      <c r="H181" t="s">
+      <c r="K181" t="s">
         <v>352</v>
-      </c>
-      <c r="K181" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="182" spans="2:19" x14ac:dyDescent="0.25">
@@ -3702,10 +3702,10 @@
         <v>35</v>
       </c>
       <c r="G185" t="s">
+        <v>270</v>
+      </c>
+      <c r="H185" t="s">
         <v>271</v>
-      </c>
-      <c r="H185" t="s">
-        <v>272</v>
       </c>
       <c r="S185" t="b">
         <v>1</v>
@@ -3807,7 +3807,7 @@
         <v>161</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4936,7 +4936,7 @@
         <v>182</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4944,7 +4944,7 @@
         <v>269</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -5139,7 +5139,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B11" t="s">
         <v>60</v>
@@ -5384,7 +5384,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B36" t="s">
         <v>48</v>
@@ -5395,7 +5395,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B37" t="s">
         <v>48</v>
@@ -5450,7 +5450,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B42" t="s">
         <v>48</v>
@@ -5494,10 +5494,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B46" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -5505,7 +5505,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B47" t="s">
         <v>50</v>
@@ -5560,7 +5560,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>

</xml_diff>